<commit_message>
finished 2 of 4 - Intro to Data Viz with Python - DataCamp
</commit_message>
<xml_diff>
--- a/Springboard Course Schedule & Study Plan.xlsx
+++ b/Springboard Course Schedule & Study Plan.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525"/>
   </bookViews>
   <sheets>
     <sheet name="Improved Dynamic Study Plan" sheetId="4" r:id="rId1"/>
     <sheet name="Dynamic Springboard Study Plan" sheetId="1" r:id="rId2"/>
     <sheet name="Springboard Study Plan" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,23 +30,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Brian Leip:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-says 10 min but actually requires 2 * 4 hour courses in python</t>
+          <t>says 10 min but actually requires 2 * 4 hour courses in python</t>
         </r>
       </text>
     </comment>
@@ -138,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="128">
   <si>
     <t>Description</t>
   </si>
@@ -446,22 +435,82 @@
     <t>Target # of months to complete course:</t>
   </si>
   <si>
-    <t>Hours Per Week (avg):</t>
-  </si>
-  <si>
     <t>Complete by</t>
   </si>
   <si>
-    <t>Week #</t>
-  </si>
-  <si>
     <t>Complete by (Max)</t>
   </si>
   <si>
     <t>Week # (Max)</t>
   </si>
   <si>
-    <t>Hours Per Day (avg):</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Work on JSON Based Data Exercises</t>
+  </si>
+  <si>
+    <t>TOTAL HOURS</t>
+  </si>
+  <si>
+    <t>HOURS COMPLETED</t>
+  </si>
+  <si>
+    <t>HOURS REMAINING</t>
+  </si>
+  <si>
+    <t>Avg Hours Per Week (ALL):</t>
+  </si>
+  <si>
+    <t>Avg Hours Per Day (ALL)</t>
+  </si>
+  <si>
+    <t>Avg Hours Per Day (REMAIN)</t>
+  </si>
+  <si>
+    <t>Avg Hours Per Week (REMAIN)</t>
+  </si>
+  <si>
+    <t>Target End Date:</t>
+  </si>
+  <si>
+    <t>Capstone Project Hours</t>
+  </si>
+  <si>
+    <t>Curriculum Hours</t>
+  </si>
+  <si>
+    <t>TOTAL HOURS FOR CERT</t>
+  </si>
+  <si>
+    <t>HOURS COMPLETED FOR CERT</t>
+  </si>
+  <si>
+    <t>HOURS REMAINING FOR CERT</t>
+  </si>
+  <si>
+    <t>Avg Hours Per Week (CERT)</t>
+  </si>
+  <si>
+    <t>Avg Hours Per Day (CERT)</t>
+  </si>
+  <si>
+    <t>Not required for cert</t>
+  </si>
+  <si>
+    <t>Curriculum Hours Required for Cert (60%)</t>
+  </si>
+  <si>
+    <t>Target months to complete:</t>
   </si>
 </sst>
 </file>
@@ -469,8 +518,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -542,7 +591,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -573,8 +622,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -658,14 +713,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -757,7 +849,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -766,13 +858,99 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="30">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1306,74 +1484,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="51.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="48" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="31" thickBot="1">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" s="14">
-        <v>4.25</v>
-      </c>
-      <c r="I1"/>
+        <v>102</v>
+      </c>
+      <c r="E1" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="49"/>
       <c r="J1" s="15" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="K1" s="37">
-        <f>$C$56/(H1*30/7)</f>
-        <v>11.369281045751633</v>
-      </c>
-      <c r="L1" s="38" t="s">
+        <f>K2*7</f>
+        <v>11.324869791666666</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="10">
         <v>43102</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="29" thickBot="1">
+      <c r="O1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1" s="58">
+        <f>ROUND((M2-M1+1)/30, 2)</f>
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22">
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="44">
         <f>5/60</f>
         <v>8.3333333333333329E-2</v>
       </c>
@@ -1384,1024 +1573,1704 @@
       <c r="E2" s="26">
         <v>1</v>
       </c>
+      <c r="F2" s="42" t="str">
+        <f ca="1">IF(G2&lt;&gt;"", "", IF(D2&lt;=TODAY(), "DUE", IF(AND(F1="DUE", D2&gt;=TODAY()), "SOON", "")))</f>
+        <v/>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="48" t="str">
+        <f ca="1">IF(AND(F2&lt;&gt;"", G2&lt;&gt;"X"), C2, "")</f>
+        <v/>
+      </c>
       <c r="J2" s="15" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="K2" s="40">
-        <f>K1/7</f>
-        <v>1.6241830065359475</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <f>C56/(M2-M1+1)</f>
+        <v>1.6178385416666665</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="10">
+        <v>43229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>2.1</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="45">
         <f>40/60</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D3" s="19">
-        <f t="shared" ref="D3:D34" si="0">D2+($C3*7/K$1)</f>
-        <v>43102.410462776657</v>
+        <f>D2+($C3/K$2)</f>
+        <v>43102.412072434607</v>
       </c>
       <c r="E3" s="20">
-        <f t="shared" ref="E3:E34" si="1">ROUNDDOWN((D3-$M$1)/7, 0)+1</f>
+        <f t="shared" ref="E3:E34" si="0">ROUNDDOWN((D3-$M$1)/7, 0)+1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="F3" s="42" t="str">
+        <f t="shared" ref="F3:F54" ca="1" si="1">IF(G3&lt;&gt;"", "", IF(D3&lt;=TODAY(), "DUE", IF(AND(F2="DUE", D3&gt;=TODAY()), "SOON", "")))</f>
+        <v/>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="48" t="str">
+        <f t="shared" ref="H3:H54" ca="1" si="2">IF(AND(F3&lt;&gt;"", G3&lt;&gt;"X"), C3, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="53">
         <v>1.5</v>
       </c>
       <c r="D4" s="19">
-        <f t="shared" si="0"/>
-        <v>43103.334004024146</v>
+        <f t="shared" ref="D4:D54" si="3">D3+($C4/K$2)</f>
+        <v>43103.339235412473</v>
       </c>
       <c r="E4" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="F4" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G4" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="40">
+        <f ca="1">K5*7</f>
+        <v>13.465789473684211</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="M4" s="40">
+        <f ca="1">M5*7</f>
+        <v>9.1749122807017525</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="46">
         <v>8</v>
       </c>
       <c r="D5" s="19">
-        <f t="shared" si="0"/>
-        <v>43108.259557344063</v>
+        <f t="shared" si="3"/>
+        <v>43108.284104627768</v>
       </c>
       <c r="E5" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="F5" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K5" s="40">
+        <f ca="1">C59/(M2-TODAY())</f>
+        <v>1.9236842105263159</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="M5" s="40">
+        <f ca="1">C69/(M2-TODAY())</f>
+        <v>1.3107017543859647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="45">
         <v>5</v>
       </c>
       <c r="D6" s="19">
-        <f t="shared" si="0"/>
-        <v>43111.338028169012</v>
+        <f t="shared" si="3"/>
+        <v>43111.374647887329</v>
       </c>
       <c r="E6" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="F6" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G6" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="45">
         <v>6</v>
       </c>
       <c r="D7" s="19">
-        <f t="shared" si="0"/>
-        <v>43115.03219315895</v>
+        <f t="shared" si="3"/>
+        <v>43115.083299798796</v>
       </c>
       <c r="E7" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="F7" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G7" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="45">
         <v>6</v>
       </c>
       <c r="D8" s="19">
-        <f t="shared" si="0"/>
-        <v>43118.726358148888</v>
+        <f t="shared" si="3"/>
+        <v>43118.791951710264</v>
       </c>
       <c r="E8" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="F8" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>DUE</v>
+      </c>
+      <c r="G8" s="60"/>
+      <c r="H8" s="48">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>3.2</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="45">
         <v>1</v>
       </c>
       <c r="D9" s="19">
-        <f t="shared" si="0"/>
-        <v>43119.342052313878</v>
+        <f t="shared" si="3"/>
+        <v>43119.410060362177</v>
       </c>
       <c r="E9" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="F9" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G9" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>3.3</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="45">
         <f>2+(5/60)</f>
         <v>2.0833333333333335</v>
       </c>
       <c r="D10" s="19">
-        <f t="shared" si="0"/>
-        <v>43120.62474849094</v>
+        <f t="shared" si="3"/>
+        <v>43120.697786720324</v>
       </c>
       <c r="E10" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="F10" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G10" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>3.4</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="53">
         <v>1</v>
       </c>
       <c r="D11" s="19">
-        <f t="shared" si="0"/>
-        <v>43121.24044265593</v>
+        <f t="shared" si="3"/>
+        <v>43121.315895372238</v>
       </c>
       <c r="E11" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="F11" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>DUE</v>
+      </c>
+      <c r="G11" s="60"/>
+      <c r="H11" s="48">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="45">
         <v>6</v>
       </c>
       <c r="D12" s="19">
-        <f t="shared" si="0"/>
-        <v>43124.934607645868</v>
+        <f t="shared" si="3"/>
+        <v>43125.024547283705</v>
       </c>
       <c r="E12" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="F12" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>DUE</v>
+      </c>
+      <c r="G12" s="60"/>
+      <c r="H12" s="48">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="45">
         <v>6</v>
       </c>
       <c r="D13" s="19">
-        <f t="shared" si="0"/>
-        <v>43128.628772635806</v>
+        <f t="shared" si="3"/>
+        <v>43128.733199195172</v>
       </c>
       <c r="E13" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="F13" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>DUE</v>
+      </c>
+      <c r="G13" s="60"/>
+      <c r="H13" s="48">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="45">
         <v>6</v>
       </c>
       <c r="D14" s="19">
-        <f t="shared" si="0"/>
-        <v>43132.322937625744</v>
+        <f t="shared" si="3"/>
+        <v>43132.44185110664</v>
       </c>
       <c r="E14" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="F14" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>DUE</v>
+      </c>
+      <c r="G14" s="60"/>
+      <c r="H14" s="48">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="45">
         <v>6</v>
       </c>
       <c r="D15" s="19">
-        <f t="shared" si="0"/>
-        <v>43136.017102615682</v>
+        <f t="shared" si="3"/>
+        <v>43136.150503018107</v>
       </c>
       <c r="E15" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="F15" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>SOON</v>
+      </c>
+      <c r="G15" s="60"/>
+      <c r="H15" s="48">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="45">
         <v>6</v>
       </c>
       <c r="D16" s="19">
-        <f t="shared" si="0"/>
-        <v>43139.71126760562</v>
+        <f t="shared" si="3"/>
+        <v>43139.859154929574</v>
       </c>
       <c r="E16" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G16" s="60"/>
+      <c r="H16" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="45">
         <v>5</v>
       </c>
       <c r="D17" s="19">
-        <f t="shared" si="0"/>
-        <v>43142.789738430569</v>
+        <f t="shared" si="3"/>
+        <v>43142.949698189135</v>
       </c>
       <c r="E17" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G17" s="60"/>
+      <c r="H17" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>60</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="45">
         <v>3</v>
       </c>
       <c r="D18" s="19">
-        <f t="shared" si="0"/>
-        <v>43144.636820925538</v>
+        <f t="shared" si="3"/>
+        <v>43144.804024144869</v>
       </c>
       <c r="E18" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G18" s="60"/>
+      <c r="H18" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="18">
+        <v>109</v>
+      </c>
+      <c r="C19" s="45">
         <v>1.5</v>
       </c>
       <c r="D19" s="19">
-        <f t="shared" si="0"/>
-        <v>43145.560362173026</v>
+        <f t="shared" si="3"/>
+        <v>43145.731187122736</v>
       </c>
       <c r="E19" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G19" s="60"/>
+      <c r="H19" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="45">
         <v>6</v>
       </c>
       <c r="D20" s="19">
-        <f t="shared" si="0"/>
-        <v>43149.254527162964</v>
+        <f t="shared" si="3"/>
+        <v>43149.439839034203</v>
       </c>
       <c r="E20" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G20" s="60"/>
+      <c r="H20" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="45">
         <v>4</v>
       </c>
       <c r="D21" s="19">
-        <f t="shared" si="0"/>
-        <v>43151.717303822923</v>
+        <f t="shared" si="3"/>
+        <v>43151.91227364185</v>
       </c>
       <c r="E21" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G21" s="60"/>
+      <c r="H21" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>65</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="45">
         <v>0.5</v>
       </c>
       <c r="D22" s="19">
-        <f t="shared" si="0"/>
-        <v>43152.025150905421</v>
+        <f t="shared" si="3"/>
+        <v>43152.221327967804</v>
       </c>
       <c r="E22" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G22" s="60"/>
+      <c r="H22" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="53">
         <v>3</v>
       </c>
       <c r="D23" s="19">
-        <f t="shared" si="0"/>
-        <v>43153.872233400391</v>
+        <f t="shared" si="3"/>
+        <v>43154.075653923537</v>
       </c>
       <c r="E23" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G23" s="60"/>
+      <c r="H23" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="45">
         <v>2</v>
       </c>
       <c r="D24" s="19">
-        <f t="shared" si="0"/>
-        <v>43155.10362173037</v>
+        <f t="shared" si="3"/>
+        <v>43155.311871227357</v>
       </c>
       <c r="E24" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G24" s="60"/>
+      <c r="H24" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="45">
         <v>2</v>
       </c>
       <c r="D25" s="19">
-        <f t="shared" si="0"/>
-        <v>43156.335010060349</v>
+        <f t="shared" si="3"/>
+        <v>43156.548088531177</v>
       </c>
       <c r="E25" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G25" s="60"/>
+      <c r="H25" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="45">
         <v>2</v>
       </c>
       <c r="D26" s="19">
-        <f t="shared" si="0"/>
-        <v>43157.566398390329</v>
+        <f t="shared" si="3"/>
+        <v>43157.784305834997</v>
       </c>
       <c r="E26" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G26" s="60"/>
+      <c r="H26" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>5.2</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="53">
         <v>10</v>
       </c>
       <c r="D27" s="19">
-        <f t="shared" si="0"/>
-        <v>43163.723340040226</v>
+        <f t="shared" si="3"/>
+        <v>43163.965392354112</v>
       </c>
       <c r="E27" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G27" s="60"/>
+      <c r="H27" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="45">
         <v>5</v>
       </c>
       <c r="D28" s="19">
-        <f t="shared" si="0"/>
-        <v>43166.801810865174</v>
+        <f t="shared" si="3"/>
+        <v>43167.055935613673</v>
       </c>
       <c r="E28" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G28" s="60"/>
+      <c r="H28" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="46">
         <v>6</v>
       </c>
       <c r="D29" s="19">
-        <f t="shared" si="0"/>
-        <v>43170.495975855112</v>
+        <f t="shared" si="3"/>
+        <v>43170.76458752514</v>
       </c>
       <c r="E29" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G29" s="60"/>
+      <c r="H29" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J29" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K29" s="57"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="46">
         <v>1.5</v>
       </c>
       <c r="D30" s="19">
-        <f t="shared" si="0"/>
-        <v>43171.4195171026</v>
+        <f t="shared" si="3"/>
+        <v>43171.691750503007</v>
       </c>
       <c r="E30" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G30" s="60"/>
+      <c r="H30" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J30" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K30" s="57"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="46">
         <v>1</v>
       </c>
       <c r="D31" s="19">
-        <f t="shared" si="0"/>
-        <v>43172.03521126759</v>
+        <f t="shared" si="3"/>
+        <v>43172.309859154921</v>
       </c>
       <c r="E31" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G31" s="60"/>
+      <c r="H31" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J31" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K31" s="57"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="46">
         <v>2</v>
       </c>
       <c r="D32" s="19">
-        <f t="shared" si="0"/>
-        <v>43173.266599597569</v>
+        <f t="shared" si="3"/>
+        <v>43173.546076458741</v>
       </c>
       <c r="E32" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="F32" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G32" s="60"/>
+      <c r="H32" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J32" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K32" s="57"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>6.3</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="46">
         <f>15/60</f>
         <v>0.25</v>
       </c>
       <c r="D33" s="19">
-        <f t="shared" si="0"/>
-        <v>43173.420523138819</v>
+        <f t="shared" si="3"/>
+        <v>43173.700603621721</v>
       </c>
       <c r="E33" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="F33" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G33" s="60"/>
+      <c r="H33" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J33" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K33" s="57"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>6.4</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="53">
         <v>6</v>
       </c>
       <c r="D34" s="19">
-        <f t="shared" si="0"/>
-        <v>43177.114688128757</v>
+        <f t="shared" si="3"/>
+        <v>43177.409255533188</v>
       </c>
       <c r="E34" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="F34" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G34" s="60"/>
+      <c r="H34" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>7</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="53">
         <v>10</v>
       </c>
       <c r="D35" s="19">
-        <f t="shared" ref="D35:D54" si="2">D34+($C35*7/K$1)</f>
-        <v>43183.271629778654</v>
+        <f t="shared" si="3"/>
+        <v>43183.590342052303</v>
       </c>
       <c r="E35" s="20">
-        <f t="shared" ref="E35:E54" si="3">ROUNDDOWN((D35-$M$1)/7, 0)+1</f>
+        <f t="shared" ref="E35:E66" si="4">ROUNDDOWN((D35-$M$1)/7, 0)+1</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="F35" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G35" s="60"/>
+      <c r="H35" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36" s="46">
         <v>3</v>
       </c>
       <c r="D36" s="19">
-        <f t="shared" si="2"/>
-        <v>43185.118712273623</v>
+        <f t="shared" si="3"/>
+        <v>43185.444668008036</v>
       </c>
       <c r="E36" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="F36" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G36" s="60"/>
+      <c r="H36" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J36" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K36" s="57"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="46">
         <v>3</v>
       </c>
       <c r="D37" s="19">
-        <f t="shared" si="2"/>
-        <v>43186.965794768592</v>
+        <f t="shared" si="3"/>
+        <v>43187.29899396377</v>
       </c>
       <c r="E37" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="F37" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G37" s="60"/>
+      <c r="H37" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J37" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K37" s="57"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="46">
         <v>3</v>
       </c>
       <c r="D38" s="19">
-        <f t="shared" si="2"/>
-        <v>43188.812877263561</v>
+        <f t="shared" si="3"/>
+        <v>43189.153319919504</v>
       </c>
       <c r="E38" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="F38" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G38" s="60"/>
+      <c r="H38" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J38" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K38" s="57"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="46">
         <v>6</v>
       </c>
       <c r="D39" s="19">
-        <f t="shared" si="2"/>
-        <v>43192.507042253499</v>
+        <f t="shared" si="3"/>
+        <v>43192.861971830971</v>
       </c>
       <c r="E39" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="F39" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G39" s="60"/>
+      <c r="H39" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J39" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K39" s="57"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C40" s="46">
         <v>3</v>
       </c>
       <c r="D40" s="19">
-        <f t="shared" si="2"/>
-        <v>43194.354124748468</v>
+        <f t="shared" si="3"/>
+        <v>43194.716297786705</v>
       </c>
       <c r="E40" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="F40" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G40" s="60"/>
+      <c r="H40" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J40" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K40" s="57"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="46">
         <v>2</v>
       </c>
       <c r="D41" s="19">
-        <f t="shared" si="2"/>
-        <v>43195.585513078448</v>
+        <f t="shared" si="3"/>
+        <v>43195.952515090525</v>
       </c>
       <c r="E41" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="I41" s="4"/>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="F41" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G41" s="60"/>
+      <c r="H41" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J41" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K41" s="57"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C42" s="46">
         <v>3</v>
       </c>
       <c r="D42" s="19">
-        <f t="shared" si="2"/>
-        <v>43197.432595573417</v>
+        <f t="shared" si="3"/>
+        <v>43197.806841046258</v>
       </c>
       <c r="E42" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="I42" s="4"/>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="F42" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G42" s="60"/>
+      <c r="H42" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J42" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K42" s="57"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="18">
+      <c r="C43" s="46">
         <v>3</v>
       </c>
       <c r="D43" s="19">
-        <f t="shared" si="2"/>
-        <v>43199.279678068386</v>
+        <f t="shared" si="3"/>
+        <v>43199.661167001992</v>
       </c>
       <c r="E43" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="F43" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G43" s="60"/>
+      <c r="H43" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J43" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K43" s="57"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="18">
+      <c r="C44" s="46">
         <v>3</v>
       </c>
       <c r="D44" s="19">
-        <f t="shared" si="2"/>
-        <v>43201.126760563355</v>
+        <f t="shared" si="3"/>
+        <v>43201.515492957726</v>
       </c>
       <c r="E44" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="F44" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G44" s="60"/>
+      <c r="H44" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J44" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K44" s="57"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="46">
         <v>2</v>
       </c>
       <c r="D45" s="19">
-        <f t="shared" si="2"/>
-        <v>43202.358148893334</v>
+        <f t="shared" si="3"/>
+        <v>43202.751710261546</v>
       </c>
       <c r="E45" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="F45" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G45" s="60"/>
+      <c r="H45" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J45" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K45" s="57"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>8.4</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="18">
+      <c r="C46" s="46">
         <v>3</v>
       </c>
       <c r="D46" s="19">
-        <f t="shared" si="2"/>
-        <v>43204.205231388303</v>
+        <f t="shared" si="3"/>
+        <v>43204.606036217279</v>
       </c>
       <c r="E46" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="F46" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G46" s="60"/>
+      <c r="H46" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J46" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K46" s="57"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C47" s="46">
         <v>3</v>
       </c>
       <c r="D47" s="19">
-        <f t="shared" si="2"/>
-        <v>43206.052313883272</v>
+        <f t="shared" si="3"/>
+        <v>43206.460362173013</v>
       </c>
       <c r="E47" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="F47" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G47" s="60"/>
+      <c r="H47" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J47" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K47" s="57"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="18">
+      <c r="C48" s="46">
         <v>6</v>
       </c>
       <c r="D48" s="19">
-        <f t="shared" si="2"/>
-        <v>43209.74647887321</v>
+        <f t="shared" si="3"/>
+        <v>43210.16901408448</v>
       </c>
       <c r="E48" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G48" s="60"/>
+      <c r="H48" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J48" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K48" s="57"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="18">
+      <c r="C49" s="46">
         <v>2</v>
       </c>
       <c r="D49" s="19">
-        <f t="shared" si="2"/>
-        <v>43210.97786720319</v>
+        <f t="shared" si="3"/>
+        <v>43211.4052313883</v>
       </c>
       <c r="E49" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G49" s="60"/>
+      <c r="H49" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="J49" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K49" s="57"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>9.1</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="18">
+      <c r="C50" s="53">
         <f>30/5</f>
         <v>6</v>
       </c>
       <c r="D50" s="19">
-        <f t="shared" si="2"/>
-        <v>43214.672032193128</v>
+        <f t="shared" si="3"/>
+        <v>43215.113883299768</v>
       </c>
       <c r="E50" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G50" s="60"/>
+      <c r="H50" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="53">
         <f>30/5</f>
         <v>6</v>
       </c>
       <c r="D51" s="19">
-        <f t="shared" si="2"/>
-        <v>43218.366197183066</v>
+        <f t="shared" si="3"/>
+        <v>43218.822535211235</v>
       </c>
       <c r="E51" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G51" s="60"/>
+      <c r="H51" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="18">
+      <c r="C52" s="53">
         <f>30/5</f>
         <v>6</v>
       </c>
       <c r="D52" s="19">
-        <f t="shared" si="2"/>
-        <v>43222.060362173004</v>
+        <f t="shared" si="3"/>
+        <v>43222.531187122702</v>
       </c>
       <c r="E52" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G52" s="60"/>
+      <c r="H52" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>9.4</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C53" s="53">
         <f>30/5</f>
         <v>6</v>
       </c>
       <c r="D53" s="19">
-        <f t="shared" si="2"/>
-        <v>43225.754527162942</v>
+        <f t="shared" si="3"/>
+        <v>43226.23983903417</v>
       </c>
       <c r="E53" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G53" s="60"/>
+      <c r="H53" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>9.5</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C54" s="18">
+      <c r="C54" s="53">
         <f>30/5</f>
         <v>6</v>
       </c>
       <c r="D54" s="19">
-        <f t="shared" si="2"/>
-        <v>43229.448692152881</v>
+        <f t="shared" si="3"/>
+        <v>43229.948490945637</v>
       </c>
       <c r="E54" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="15" thickBot="1">
-      <c r="C56" s="39">
+      <c r="F54" s="42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G54" s="60"/>
+      <c r="H54" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="47">
         <f>SUM(C1:C55)</f>
         <v>207.08333333333331</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15" thickTop="1"/>
+    <row r="57" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="50"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="51">
+        <f>C56-C59</f>
+        <v>24.333333333333314</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" s="51">
+        <f>SUMIF(G2:G54, "", C2:C54)</f>
+        <v>182.75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" s="53">
+        <f>SUM(C50:C54,C34:C35, C27, C23, C11, C4)</f>
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" s="45">
+        <f>C56-C62</f>
+        <v>145.58333333333331</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" s="45">
+        <f>C63*0.6</f>
+        <v>87.34999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="C66" s="47">
+        <f>C62+C64</f>
+        <v>148.84999999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="50"/>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C68" s="51">
+        <f>C58</f>
+        <v>24.333333333333314</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" s="51">
+        <f>C66-C68</f>
+        <v>124.51666666666665</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2414,32 +3283,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="51.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.6640625" style="36" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" customWidth="1"/>
-    <col min="14" max="14" width="4.1640625" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" customWidth="1"/>
-    <col min="16" max="16" width="4.1640625" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.7109375" style="36" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="31" thickBot="1">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>2</v>
       </c>
@@ -2457,10 +3328,10 @@
       </c>
       <c r="F1" s="33"/>
       <c r="G1" s="30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>101</v>
@@ -2489,7 +3360,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -2516,7 +3387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2.1</v>
       </c>
@@ -2545,7 +3416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>2.2000000000000002</v>
       </c>
@@ -2573,7 +3444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
@@ -2601,7 +3472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -2629,7 +3500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
@@ -2657,7 +3528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -2685,7 +3556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>3.2</v>
       </c>
@@ -2713,7 +3584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>3.3</v>
       </c>
@@ -2742,7 +3613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>3.4</v>
       </c>
@@ -2770,7 +3641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
@@ -2798,7 +3669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
@@ -2826,7 +3697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -2854,7 +3725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>27</v>
       </c>
@@ -2882,7 +3753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>58</v>
       </c>
@@ -2910,7 +3781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>59</v>
       </c>
@@ -2938,7 +3809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>60</v>
       </c>
@@ -2966,7 +3837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>61</v>
       </c>
@@ -2994,7 +3865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
@@ -3022,7 +3893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>64</v>
       </c>
@@ -3050,7 +3921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>65</v>
       </c>
@@ -3078,7 +3949,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>67</v>
       </c>
@@ -3106,7 +3977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>69</v>
       </c>
@@ -3134,7 +4005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>70</v>
       </c>
@@ -3162,7 +4033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>71</v>
       </c>
@@ -3190,7 +4061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>5.2</v>
       </c>
@@ -3218,7 +4089,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>72</v>
       </c>
@@ -3246,7 +4117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>73</v>
       </c>
@@ -3274,7 +4145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>74</v>
       </c>
@@ -3302,7 +4173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>75</v>
       </c>
@@ -3330,7 +4201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>76</v>
       </c>
@@ -3358,7 +4229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>6.3</v>
       </c>
@@ -3387,7 +4258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>6.4</v>
       </c>
@@ -3415,7 +4286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>7</v>
       </c>
@@ -3443,7 +4314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
@@ -3471,7 +4342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>80</v>
       </c>
@@ -3499,7 +4370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>81</v>
       </c>
@@ -3527,7 +4398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
@@ -3555,7 +4426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>84</v>
       </c>
@@ -3583,7 +4454,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>86</v>
       </c>
@@ -3611,7 +4482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>88</v>
       </c>
@@ -3639,7 +4510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>89</v>
       </c>
@@ -3667,7 +4538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>90</v>
       </c>
@@ -3695,7 +4566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>91</v>
       </c>
@@ -3723,7 +4594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>8.4</v>
       </c>
@@ -3751,7 +4622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>93</v>
       </c>
@@ -3779,7 +4650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>94</v>
       </c>
@@ -3807,7 +4678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>95</v>
       </c>
@@ -3835,7 +4706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>9.1</v>
       </c>
@@ -3864,7 +4735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>9.1999999999999993</v>
       </c>
@@ -3893,7 +4764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>9.3000000000000007</v>
       </c>
@@ -3922,7 +4793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>9.4</v>
       </c>
@@ -3951,7 +4822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>9.5</v>
       </c>
@@ -3980,13 +4851,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15" thickBot="1">
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="39">
         <f>SUM(C1:C55)</f>
         <v>207.08333333333331</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15" thickTop="1"/>
+    <row r="57" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
@@ -4007,24 +4878,24 @@
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="15:16">
+    <row r="1" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O1" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="15:16">
+    <row r="2" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O2" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="15:16">
+    <row r="3" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O3" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="15:16">
+    <row r="4" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O4" s="4">
         <v>43132</v>
       </c>

</xml_diff>

<commit_message>
progress on ch 3 of 4 - Data Viz with Python - DataCamp
</commit_message>
<xml_diff>
--- a/Springboard Course Schedule & Study Plan.xlsx
+++ b/Springboard Course Schedule & Study Plan.xlsx
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="128">
   <si>
     <t>Description</t>
   </si>
@@ -1488,7 +1488,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,14 +1663,14 @@
       </c>
       <c r="K4" s="40">
         <f ca="1">K5*7</f>
-        <v>13.60904255319149</v>
+        <v>13.68010752688172</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>123</v>
       </c>
       <c r="M4" s="40">
         <f ca="1">M5*7</f>
-        <v>9.2725177304964532</v>
+        <v>9.2969534050179199</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1707,14 +1707,14 @@
       </c>
       <c r="K5" s="40">
         <f ca="1">C59/(M2-TODAY())</f>
-        <v>1.9441489361702127</v>
+        <v>1.9543010752688172</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>124</v>
       </c>
       <c r="M5" s="40">
         <f ca="1">C69/(M2-TODAY())</f>
-        <v>1.3246453900709219</v>
+        <v>1.3281362007168458</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1886,12 +1886,14 @@
       </c>
       <c r="F11" s="42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DUE</v>
-      </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="48">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v/>
+      </c>
+      <c r="G11" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" s="48" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -3198,7 +3200,7 @@
       </c>
       <c r="C58" s="51">
         <f>C56-C59</f>
-        <v>24.333333333333314</v>
+        <v>25.333333333333314</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3207,7 +3209,7 @@
       </c>
       <c r="C59" s="51">
         <f>SUMIF(G2:G54, "", C2:C54)</f>
-        <v>182.75</v>
+        <v>181.75</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3255,7 +3257,7 @@
       </c>
       <c r="C68" s="51">
         <f>C58</f>
-        <v>24.333333333333314</v>
+        <v>25.333333333333314</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -3264,7 +3266,7 @@
       </c>
       <c r="C69" s="51">
         <f>C66-C68</f>
-        <v>124.51666666666665</v>
+        <v>123.51666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Capstone Project Proposal including suggestions from Nate
</commit_message>
<xml_diff>
--- a/Springboard Course Schedule & Study Plan.xlsx
+++ b/Springboard Course Schedule & Study Plan.xlsx
@@ -1488,7 +1488,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,14 +1663,14 @@
       </c>
       <c r="K4" s="40">
         <f ca="1">K5*7</f>
-        <v>13.68010752688172</v>
+        <v>13.828804347826088</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>123</v>
       </c>
       <c r="M4" s="40">
         <f ca="1">M5*7</f>
-        <v>9.2969534050179199</v>
+        <v>9.3980072463768103</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1707,14 +1707,14 @@
       </c>
       <c r="K5" s="40">
         <f ca="1">C59/(M2-TODAY())</f>
-        <v>1.9543010752688172</v>
+        <v>1.9755434782608696</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>124</v>
       </c>
       <c r="M5" s="40">
         <f ca="1">C69/(M2-TODAY())</f>
-        <v>1.3281362007168458</v>
+        <v>1.3425724637681158</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="F15" s="42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SOON</v>
+        <v>DUE</v>
       </c>
       <c r="G15" s="60"/>
       <c r="H15" s="48">
@@ -2028,12 +2028,12 @@
       </c>
       <c r="F16" s="42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>SOON</v>
       </c>
       <c r="G16" s="60"/>
-      <c r="H16" s="48" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+      <c r="H16" s="48">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
progress on data viz
</commit_message>
<xml_diff>
--- a/Springboard Course Schedule & Study Plan.xlsx
+++ b/Springboard Course Schedule & Study Plan.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Improved Dynamic Study Plan" sheetId="4" r:id="rId1"/>
     <sheet name="Dynamic Springboard Study Plan" sheetId="1" r:id="rId2"/>
     <sheet name="Springboard Study Plan" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="138">
   <si>
     <t>Description</t>
   </si>
@@ -511,6 +511,36 @@
   </si>
   <si>
     <t>Target months to complete:</t>
+  </si>
+  <si>
+    <t>Avg Hours Per Week (REMAIN +50%)</t>
+  </si>
+  <si>
+    <t>Avg Hours Per Day (REMAIN+50%)</t>
+  </si>
+  <si>
+    <t>Avg Hours Per Week (CERT+50%)</t>
+  </si>
+  <si>
+    <t>Avg Hours Per Day (CERT+50%)</t>
+  </si>
+  <si>
+    <t>LEGEND:</t>
+  </si>
+  <si>
+    <t>ALL = 100% of course, completed between Start date and Target End Date</t>
+  </si>
+  <si>
+    <t>REMAIN = 100% of the course, spreading the remaining hours between today and the Target End Date</t>
+  </si>
+  <si>
+    <t>CERT = Requirements for the course certificate (100% projects, 60% curriculum) completed between today and Target End Date</t>
+  </si>
+  <si>
+    <t>+50% = Springboard recommends allocating 50% additional time to the suggested hours, especially if the topic is new to you</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note - The "Complete by" dates use the ALL method.  </t>
   </si>
 </sst>
 </file>
@@ -518,10 +548,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +620,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -629,7 +667,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -724,11 +762,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -757,7 +864,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -849,7 +956,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -858,7 +965,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -867,37 +974,37 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -921,6 +1028,24 @@
     <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="30">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1484,34 +1609,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="61" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="48" customWidth="1"/>
-    <col min="9" max="9" width="2.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="5.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="6.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" style="48" customWidth="1"/>
+    <col min="9" max="9" width="2.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.7109375" customWidth="1"/>
+    <col min="14" max="14" width="2.6640625" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" customWidth="1"/>
+    <col min="16" max="16" width="5.83203125" customWidth="1"/>
+    <col min="17" max="17" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="31" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>2</v>
       </c>
@@ -1555,7 +1681,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="29" thickBot="1">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -1598,7 +1724,7 @@
         <v>43229</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15" thickBot="1">
       <c r="A3" s="16">
         <v>2.1</v>
       </c>
@@ -1610,7 +1736,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D3" s="19">
-        <f>D2+($C3/K$2)</f>
+        <f>D2+$C3/K$2</f>
         <v>43102.412072434607</v>
       </c>
       <c r="E3" s="20">
@@ -1629,7 +1755,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="29" thickBot="1">
       <c r="A4" s="16">
         <v>2.2000000000000002</v>
       </c>
@@ -1640,7 +1766,7 @@
         <v>1.5</v>
       </c>
       <c r="D4" s="19">
-        <f t="shared" ref="D4:D54" si="3">D3+($C4/K$2)</f>
+        <f t="shared" ref="D4:D54" si="3">D3+$C4/K$2</f>
         <v>43103.339235412473</v>
       </c>
       <c r="E4" s="20">
@@ -1663,17 +1789,17 @@
       </c>
       <c r="K4" s="40">
         <f ca="1">K5*7</f>
-        <v>13.828804347826088</v>
+        <v>13.98076923076923</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>123</v>
       </c>
       <c r="M4" s="40">
         <f ca="1">M5*7</f>
-        <v>9.3980072463768103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>9.5012820512820504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="29" thickBot="1">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
@@ -1707,17 +1833,17 @@
       </c>
       <c r="K5" s="40">
         <f ca="1">C59/(M2-TODAY())</f>
-        <v>1.9755434782608696</v>
+        <v>1.9972527472527473</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>124</v>
       </c>
       <c r="M5" s="40">
         <f ca="1">C69/(M2-TODAY())</f>
-        <v>1.3425724637681158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1.3573260073260072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" thickBot="1">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -1747,7 +1873,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="29" thickBot="1">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
@@ -1776,8 +1902,22 @@
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J7" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="K7" s="40">
+        <f ca="1">+K4*1.5</f>
+        <v>20.971153846153847</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="M7" s="40">
+        <f ca="1">+M4*1.5</f>
+        <v>14.251923076923076</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="29" thickBot="1">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -1804,8 +1944,22 @@
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J8" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="K8" s="40">
+        <f ca="1">+K5*1.5</f>
+        <v>2.9958791208791209</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="M8" s="40">
+        <f ca="1">+M5*1.5</f>
+        <v>2.0359890109890109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="16">
         <v>3.2</v>
       </c>
@@ -1835,7 +1989,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" s="16">
         <v>3.3</v>
       </c>
@@ -1866,7 +2020,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="16">
         <v>3.4</v>
       </c>
@@ -1895,8 +2049,11 @@
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J11" s="73" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
@@ -1923,8 +2080,18 @@
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J12" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="65"/>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1951,8 +2118,18 @@
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J13" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="68"/>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -1979,8 +2156,18 @@
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J14" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="67"/>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="68"/>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="16" t="s">
         <v>27</v>
       </c>
@@ -2007,8 +2194,18 @@
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J15" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="71"/>
+      <c r="N15" s="71"/>
+      <c r="O15" s="71"/>
+      <c r="P15" s="71"/>
+      <c r="Q15" s="72"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="16" t="s">
         <v>58</v>
       </c>
@@ -2036,7 +2233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="16" t="s">
         <v>59</v>
       </c>
@@ -2063,8 +2260,11 @@
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="74" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="16" t="s">
         <v>60</v>
       </c>
@@ -2092,7 +2292,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="16" t="s">
         <v>61</v>
       </c>
@@ -2120,7 +2320,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
@@ -2148,7 +2348,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="16" t="s">
         <v>64</v>
       </c>
@@ -2176,7 +2376,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="16" t="s">
         <v>65</v>
       </c>
@@ -2204,7 +2404,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="16" t="s">
         <v>67</v>
       </c>
@@ -2232,7 +2432,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="16" t="s">
         <v>69</v>
       </c>
@@ -2260,7 +2460,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="16" t="s">
         <v>70</v>
       </c>
@@ -2288,7 +2488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="16" t="s">
         <v>71</v>
       </c>
@@ -2316,7 +2516,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="16">
         <v>5.2</v>
       </c>
@@ -2344,7 +2544,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="16" t="s">
         <v>72</v>
       </c>
@@ -2372,7 +2572,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="16" t="s">
         <v>73</v>
       </c>
@@ -2404,7 +2604,7 @@
       </c>
       <c r="K29" s="57"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="16" t="s">
         <v>74</v>
       </c>
@@ -2436,7 +2636,7 @@
       </c>
       <c r="K30" s="57"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="16" t="s">
         <v>75</v>
       </c>
@@ -2468,7 +2668,7 @@
       </c>
       <c r="K31" s="57"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="16" t="s">
         <v>76</v>
       </c>
@@ -2500,7 +2700,7 @@
       </c>
       <c r="K32" s="57"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="16">
         <v>6.3</v>
       </c>
@@ -2533,7 +2733,7 @@
       </c>
       <c r="K33" s="57"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="16">
         <v>6.4</v>
       </c>
@@ -2561,7 +2761,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="16">
         <v>7</v>
       </c>
@@ -2589,7 +2789,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
@@ -2621,7 +2821,7 @@
       </c>
       <c r="K36" s="57"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="16" t="s">
         <v>80</v>
       </c>
@@ -2653,7 +2853,7 @@
       </c>
       <c r="K37" s="57"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="16" t="s">
         <v>81</v>
       </c>
@@ -2685,7 +2885,7 @@
       </c>
       <c r="K38" s="57"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
@@ -2717,7 +2917,7 @@
       </c>
       <c r="K39" s="57"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="16" t="s">
         <v>84</v>
       </c>
@@ -2749,7 +2949,7 @@
       </c>
       <c r="K40" s="57"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="16" t="s">
         <v>86</v>
       </c>
@@ -2781,7 +2981,7 @@
       </c>
       <c r="K41" s="57"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="16" t="s">
         <v>88</v>
       </c>
@@ -2813,7 +3013,7 @@
       </c>
       <c r="K42" s="57"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="16" t="s">
         <v>89</v>
       </c>
@@ -2845,7 +3045,7 @@
       </c>
       <c r="K43" s="57"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44" s="16" t="s">
         <v>90</v>
       </c>
@@ -2877,7 +3077,7 @@
       </c>
       <c r="K44" s="57"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45" s="16" t="s">
         <v>91</v>
       </c>
@@ -2909,7 +3109,7 @@
       </c>
       <c r="K45" s="57"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" s="16">
         <v>8.4</v>
       </c>
@@ -2941,7 +3141,7 @@
       </c>
       <c r="K46" s="57"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47" s="16" t="s">
         <v>93</v>
       </c>
@@ -2973,7 +3173,7 @@
       </c>
       <c r="K47" s="57"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48" s="16" t="s">
         <v>94</v>
       </c>
@@ -3005,7 +3205,7 @@
       </c>
       <c r="K48" s="57"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="A49" s="16" t="s">
         <v>95</v>
       </c>
@@ -3037,7 +3237,7 @@
       </c>
       <c r="K49" s="57"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="A50" s="16">
         <v>9.1</v>
       </c>
@@ -3066,7 +3266,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="A51" s="16">
         <v>9.1999999999999993</v>
       </c>
@@ -3095,7 +3295,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="A52" s="16">
         <v>9.3000000000000007</v>
       </c>
@@ -3124,7 +3324,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53" s="16">
         <v>9.4</v>
       </c>
@@ -3153,7 +3353,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="A54" s="16">
         <v>9.5</v>
       </c>
@@ -3182,7 +3382,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="15" thickBot="1">
       <c r="B56" s="50" t="s">
         <v>110</v>
       </c>
@@ -3191,10 +3391,10 @@
         <v>207.08333333333331</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="15" thickTop="1">
       <c r="B57" s="50"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11">
       <c r="B58" s="50" t="s">
         <v>111</v>
       </c>
@@ -3203,7 +3403,7 @@
         <v>25.333333333333314</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11">
       <c r="B59" s="50" t="s">
         <v>112</v>
       </c>
@@ -3212,7 +3412,7 @@
         <v>181.75</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11">
       <c r="B62" s="55" t="s">
         <v>118</v>
       </c>
@@ -3221,7 +3421,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11">
       <c r="B63" s="52" t="s">
         <v>119</v>
       </c>
@@ -3230,7 +3430,7 @@
         <v>145.58333333333331</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11">
       <c r="B64" s="52" t="s">
         <v>126</v>
       </c>
@@ -3239,7 +3439,7 @@
         <v>87.34999999999998</v>
       </c>
     </row>
-    <row r="66" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:3" ht="15" thickBot="1">
       <c r="B66" s="50" t="s">
         <v>120</v>
       </c>
@@ -3248,10 +3448,10 @@
         <v>148.84999999999997</v>
       </c>
     </row>
-    <row r="67" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" ht="15" thickTop="1">
       <c r="B67" s="50"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3">
       <c r="B68" s="50" t="s">
         <v>121</v>
       </c>
@@ -3260,7 +3460,7 @@
         <v>25.333333333333314</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3">
       <c r="B69" s="50" t="s">
         <v>122</v>
       </c>
@@ -3271,8 +3471,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3286,33 +3486,33 @@
   <dimension ref="A1:R57"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" style="36" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="46.5" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.6640625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="46" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>2</v>
       </c>
@@ -3362,7 +3562,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -3389,7 +3589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" s="16">
         <v>2.1</v>
       </c>
@@ -3418,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="A4" s="16">
         <v>2.2000000000000002</v>
       </c>
@@ -3446,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
@@ -3474,7 +3674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -3502,7 +3702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
@@ -3530,7 +3730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -3558,7 +3758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9" s="16">
         <v>3.2</v>
       </c>
@@ -3586,7 +3786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" s="16">
         <v>3.3</v>
       </c>
@@ -3615,7 +3815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" s="16">
         <v>3.4</v>
       </c>
@@ -3643,7 +3843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
@@ -3671,7 +3871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
@@ -3699,7 +3899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -3727,7 +3927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15" s="16" t="s">
         <v>27</v>
       </c>
@@ -3755,7 +3955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="A16" s="16" t="s">
         <v>58</v>
       </c>
@@ -3783,7 +3983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="16" t="s">
         <v>59</v>
       </c>
@@ -3811,7 +4011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="16" t="s">
         <v>60</v>
       </c>
@@ -3839,7 +4039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="16" t="s">
         <v>61</v>
       </c>
@@ -3867,7 +4067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
@@ -3895,7 +4095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="16" t="s">
         <v>64</v>
       </c>
@@ -3923,7 +4123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="16" t="s">
         <v>65</v>
       </c>
@@ -3951,7 +4151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="16" t="s">
         <v>67</v>
       </c>
@@ -3979,7 +4179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="16" t="s">
         <v>69</v>
       </c>
@@ -4007,7 +4207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="16" t="s">
         <v>70</v>
       </c>
@@ -4035,7 +4235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="16" t="s">
         <v>71</v>
       </c>
@@ -4063,7 +4263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="16">
         <v>5.2</v>
       </c>
@@ -4091,7 +4291,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="16" t="s">
         <v>72</v>
       </c>
@@ -4119,7 +4319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="16" t="s">
         <v>73</v>
       </c>
@@ -4147,7 +4347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="16" t="s">
         <v>74</v>
       </c>
@@ -4175,7 +4375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
         <v>75</v>
       </c>
@@ -4203,7 +4403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="16" t="s">
         <v>76</v>
       </c>
@@ -4231,7 +4431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="16">
         <v>6.3</v>
       </c>
@@ -4260,7 +4460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="16">
         <v>6.4</v>
       </c>
@@ -4288,7 +4488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="16">
         <v>7</v>
       </c>
@@ -4316,7 +4516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
@@ -4344,7 +4544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="16" t="s">
         <v>80</v>
       </c>
@@ -4372,7 +4572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="16" t="s">
         <v>81</v>
       </c>
@@ -4400,7 +4600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
@@ -4428,7 +4628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="16" t="s">
         <v>84</v>
       </c>
@@ -4456,7 +4656,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="16" t="s">
         <v>86</v>
       </c>
@@ -4484,7 +4684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="16" t="s">
         <v>88</v>
       </c>
@@ -4512,7 +4712,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="16" t="s">
         <v>89</v>
       </c>
@@ -4540,7 +4740,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="16" t="s">
         <v>90</v>
       </c>
@@ -4568,7 +4768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="16" t="s">
         <v>91</v>
       </c>
@@ -4596,7 +4796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="16">
         <v>8.4</v>
       </c>
@@ -4624,7 +4824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="16" t="s">
         <v>93</v>
       </c>
@@ -4652,7 +4852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="16" t="s">
         <v>94</v>
       </c>
@@ -4680,7 +4880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="16" t="s">
         <v>95</v>
       </c>
@@ -4708,7 +4908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="16">
         <v>9.1</v>
       </c>
@@ -4737,7 +4937,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="16">
         <v>9.1999999999999993</v>
       </c>
@@ -4766,7 +4966,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="16">
         <v>9.3000000000000007</v>
       </c>
@@ -4795,7 +4995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="16">
         <v>9.4</v>
       </c>
@@ -4824,7 +5024,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="16">
         <v>9.5</v>
       </c>
@@ -4853,13 +5053,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="15" thickBot="1">
       <c r="C56" s="39">
         <f>SUM(C1:C55)</f>
         <v>207.08333333333331</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:8" ht="15" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
@@ -4876,28 +5076,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="15:16">
       <c r="O1" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="15:16">
       <c r="O2" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="15:16">
       <c r="O3" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="15:16">
       <c r="O4" s="4">
         <v>43132</v>
       </c>

</xml_diff>

<commit_message>
finished ch 3 of 4 Data Viz with Python on DataCamp
</commit_message>
<xml_diff>
--- a/Springboard Course Schedule & Study Plan.xlsx
+++ b/Springboard Course Schedule & Study Plan.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525"/>
   </bookViews>
   <sheets>
     <sheet name="Improved Dynamic Study Plan" sheetId="4" r:id="rId1"/>
     <sheet name="Dynamic Springboard Study Plan" sheetId="1" r:id="rId2"/>
     <sheet name="Springboard Study Plan" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -548,8 +548,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -835,7 +835,7 @@
   <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -956,7 +956,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -965,7 +965,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -974,37 +974,37 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1613,31 +1613,31 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="6.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" style="61" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" style="48" customWidth="1"/>
-    <col min="9" max="9" width="2.6640625" customWidth="1"/>
-    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="61" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="48" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.6640625" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="5.83203125" customWidth="1"/>
-    <col min="17" max="17" width="31.5" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" customWidth="1"/>
+    <col min="17" max="17" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="31" thickBot="1">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>2</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29" thickBot="1">
+    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>43229</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" thickBot="1">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>2.1</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="29" thickBot="1">
+    <row r="4" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>2.2000000000000002</v>
       </c>
@@ -1789,17 +1789,17 @@
       </c>
       <c r="K4" s="40">
         <f ca="1">K5*7</f>
-        <v>13.98076923076923</v>
+        <v>14.136111111111111</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>123</v>
       </c>
       <c r="M4" s="40">
         <f ca="1">M5*7</f>
-        <v>9.5012820512820504</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="29" thickBot="1">
+        <v>9.6068518518518502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
@@ -1833,17 +1833,17 @@
       </c>
       <c r="K5" s="40">
         <f ca="1">C59/(M2-TODAY())</f>
-        <v>1.9972527472527473</v>
+        <v>2.0194444444444444</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>124</v>
       </c>
       <c r="M5" s="40">
         <f ca="1">C69/(M2-TODAY())</f>
-        <v>1.3573260073260072</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1">
+        <v>1.3724074074074073</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="29" thickBot="1">
+    <row r="7" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
@@ -1907,17 +1907,17 @@
       </c>
       <c r="K7" s="40">
         <f ca="1">+K4*1.5</f>
-        <v>20.971153846153847</v>
+        <v>21.204166666666666</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>130</v>
       </c>
       <c r="M7" s="40">
         <f ca="1">+M4*1.5</f>
-        <v>14.251923076923076</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="29" thickBot="1">
+        <v>14.410277777777775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -1949,17 +1949,17 @@
       </c>
       <c r="K8" s="40">
         <f ca="1">+K5*1.5</f>
-        <v>2.9958791208791209</v>
+        <v>3.0291666666666668</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>131</v>
       </c>
       <c r="M8" s="40">
         <f ca="1">+M5*1.5</f>
-        <v>2.0359890109890109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>2.0586111111111109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>3.2</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>3.3</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>3.4</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="P12" s="64"/>
       <c r="Q12" s="65"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
@@ -2129,7 +2129,7 @@
       <c r="P13" s="67"/>
       <c r="Q13" s="68"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -2167,7 +2167,7 @@
       <c r="P14" s="67"/>
       <c r="Q14" s="68"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>27</v>
       </c>
@@ -2205,7 +2205,7 @@
       <c r="P15" s="71"/>
       <c r="Q15" s="72"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>58</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>59</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>60</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>61</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>64</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>65</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>67</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>69</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>70</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>71</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>5.2</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>72</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>73</v>
       </c>
@@ -2604,7 +2604,7 @@
       </c>
       <c r="K29" s="57"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>74</v>
       </c>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="K30" s="57"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>75</v>
       </c>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="K31" s="57"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>76</v>
       </c>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="K32" s="57"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>6.3</v>
       </c>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="K33" s="57"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>6.4</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>7</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="K36" s="57"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>80</v>
       </c>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="K37" s="57"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>81</v>
       </c>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="K38" s="57"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="K39" s="57"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>84</v>
       </c>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="K40" s="57"/>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>86</v>
       </c>
@@ -2981,7 +2981,7 @@
       </c>
       <c r="K41" s="57"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>88</v>
       </c>
@@ -3013,7 +3013,7 @@
       </c>
       <c r="K42" s="57"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>89</v>
       </c>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="K43" s="57"/>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>90</v>
       </c>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="K44" s="57"/>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>91</v>
       </c>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="K45" s="57"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>8.4</v>
       </c>
@@ -3141,7 +3141,7 @@
       </c>
       <c r="K46" s="57"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>93</v>
       </c>
@@ -3173,7 +3173,7 @@
       </c>
       <c r="K47" s="57"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>94</v>
       </c>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="K48" s="57"/>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>95</v>
       </c>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="K49" s="57"/>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>9.1</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>9.1999999999999993</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>9.3000000000000007</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>9.4</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>9.5</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="50" t="s">
         <v>110</v>
       </c>
@@ -3391,10 +3391,10 @@
         <v>207.08333333333331</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15" thickTop="1">
+    <row r="57" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B57" s="50"/>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B58" s="50" t="s">
         <v>111</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>25.333333333333314</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59" s="50" t="s">
         <v>112</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>181.75</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" s="55" t="s">
         <v>118</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="52" t="s">
         <v>119</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>145.58333333333331</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" s="52" t="s">
         <v>126</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>87.34999999999998</v>
       </c>
     </row>
-    <row r="66" spans="2:3" ht="15" thickBot="1">
+    <row r="66" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="50" t="s">
         <v>120</v>
       </c>
@@ -3448,10 +3448,10 @@
         <v>148.84999999999997</v>
       </c>
     </row>
-    <row r="67" spans="2:3" ht="15" thickTop="1">
+    <row r="67" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B67" s="50"/>
     </row>
-    <row r="68" spans="2:3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="50" t="s">
         <v>121</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>25.333333333333314</v>
       </c>
     </row>
-    <row r="69" spans="2:3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="50" t="s">
         <v>122</v>
       </c>
@@ -3490,29 +3490,29 @@
       <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.6640625" style="36" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.83203125" customWidth="1"/>
-    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.7109375" style="36" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="46" thickBot="1">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>2</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2.1</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>2.2000000000000002</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>3.2</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>3.3</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>3.4</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>27</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>58</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>59</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>60</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>61</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>64</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>65</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>67</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>69</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>70</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>71</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>5.2</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>72</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>73</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>74</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>75</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>76</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>6.3</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>6.4</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>7</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>80</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>81</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>84</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>86</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>88</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>89</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>90</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>91</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>8.4</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>93</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>94</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>95</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>9.1</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>9.1999999999999993</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>9.3000000000000007</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>9.4</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>9.5</v>
       </c>
@@ -5053,13 +5053,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15" thickBot="1">
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="39">
         <f>SUM(C1:C55)</f>
         <v>207.08333333333331</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15" thickTop="1"/>
+    <row r="57" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
@@ -5080,24 +5080,24 @@
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="15:16">
+    <row r="1" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O1" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="15:16">
+    <row r="2" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O2" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="15:16">
+    <row r="3" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O3" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="15:16">
+    <row r="4" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O4" s="4">
         <v>43132</v>
       </c>

</xml_diff>

<commit_message>
Finished ch 1 of 4 - pandas Foundations - DataCamp
</commit_message>
<xml_diff>
--- a/Springboard Course Schedule & Study Plan.xlsx
+++ b/Springboard Course Schedule & Study Plan.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525"/>
   </bookViews>
   <sheets>
     <sheet name="Improved Dynamic Study Plan" sheetId="4" r:id="rId1"/>
     <sheet name="Dynamic Springboard Study Plan" sheetId="1" r:id="rId2"/>
     <sheet name="Springboard Study Plan" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="139">
   <si>
     <t>Description</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t xml:space="preserve">Note - The "Complete by" dates use the ALL method.  </t>
+  </si>
+  <si>
+    <t>Customize by changing blue cells</t>
   </si>
 </sst>
 </file>
@@ -548,8 +551,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -667,7 +670,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -831,11 +834,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -865,7 +883,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -957,16 +975,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -975,37 +990,37 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1047,6 +1062,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1615,82 +1639,82 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="6.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" style="61" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" style="48" customWidth="1"/>
-    <col min="9" max="9" width="2.6640625" customWidth="1"/>
-    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="47" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.6640625" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="5.83203125" customWidth="1"/>
-    <col min="17" max="17" width="31.5" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" customWidth="1"/>
+    <col min="17" max="17" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="31" thickBot="1">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="49"/>
+      <c r="H1" s="48"/>
       <c r="J1" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="K1" s="37">
+      <c r="K1" s="74">
         <f>K2*7</f>
-        <v>11.324869791666666</v>
+        <v>11.980027548209366</v>
       </c>
       <c r="L1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="10">
+      <c r="M1" s="75">
         <v>43102</v>
       </c>
       <c r="O1" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="P1" s="58">
+      <c r="P1" s="57">
         <f>ROUND((M2-M1+1)/30, 2)</f>
-        <v>4.2699999999999996</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="29" thickBot="1">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22">
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="43">
         <f>5/60</f>
         <v>8.3333333333333329E-2</v>
       </c>
@@ -1701,1778 +1725,1780 @@
       <c r="E2" s="26">
         <v>1</v>
       </c>
-      <c r="F2" s="42" t="str">
+      <c r="F2" s="41" t="str">
         <f ca="1">IF(G2&lt;&gt;"", "", IF(D2&lt;=TODAY(), "DUE", IF(AND(F1="DUE", D2&gt;=TODAY()), "SOON", "")))</f>
         <v/>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="48" t="str">
+      <c r="H2" s="47" t="str">
         <f ca="1">IF(AND(F2&lt;&gt;"", G2&lt;&gt;"X"), C2, "")</f>
         <v/>
       </c>
       <c r="J2" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="K2" s="40">
+      <c r="K2" s="39">
         <f>C56/(M2-M1+1)</f>
-        <v>1.6178385416666665</v>
-      </c>
-      <c r="L2" s="38" t="s">
+        <v>1.7114325068870522</v>
+      </c>
+      <c r="L2" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="M2" s="10">
-        <v>43229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15" thickBot="1">
+      <c r="M2" s="75">
+        <v>43222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>2.1</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="44">
         <f>40/60</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D3" s="19">
         <f>D2+$C3/K$2</f>
-        <v>43102.412072434607</v>
+        <v>43102.389537223338</v>
       </c>
       <c r="E3" s="20">
         <f t="shared" ref="E3:E34" si="0">ROUNDDOWN((D3-$M$1)/7, 0)+1</f>
         <v>1</v>
       </c>
-      <c r="F3" s="42" t="str">
+      <c r="F3" s="41" t="str">
         <f t="shared" ref="F3:F54" ca="1" si="1">IF(G3&lt;&gt;"", "", IF(D3&lt;=TODAY(), "DUE", IF(AND(F2="DUE", D3&gt;=TODAY()), "SOON", "")))</f>
         <v/>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="48" t="str">
+      <c r="H3" s="47" t="str">
         <f t="shared" ref="H3:H54" ca="1" si="2">IF(AND(F3&lt;&gt;"", G3&lt;&gt;"X"), C3, "")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="29" thickBot="1">
+    <row r="4" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="53">
+      <c r="C4" s="52">
         <v>1.5</v>
       </c>
       <c r="D4" s="19">
         <f t="shared" ref="D4:D54" si="3">D3+$C4/K$2</f>
-        <v>43103.339235412473</v>
+        <v>43103.265995975853</v>
       </c>
       <c r="E4" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F4" s="42" t="str">
+      <c r="F4" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H4" s="48" t="str">
+      <c r="H4" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="J4" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="40">
+      <c r="K4" s="39">
         <f ca="1">K5*7</f>
-        <v>13.351123595505618</v>
+        <v>15.188271604938272</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="M4" s="40">
+      <c r="M4" s="39">
         <f ca="1">M5*7</f>
-        <v>8.7709737827715344</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="29" thickBot="1">
+        <v>10.155761316872427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>8</v>
       </c>
       <c r="D5" s="19">
         <f t="shared" si="3"/>
-        <v>43108.284104627768</v>
+        <v>43107.940442655934</v>
       </c>
       <c r="E5" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F5" s="42" t="str">
+      <c r="F5" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H5" s="48" t="str">
+      <c r="H5" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="J5" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K5" s="40">
+      <c r="K5" s="39">
         <f ca="1">C59/(M2-TODAY())</f>
-        <v>1.9073033707865168</v>
+        <v>2.1697530864197532</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="M5" s="40">
+      <c r="M5" s="39">
         <f ca="1">C69/(M2-TODAY())</f>
-        <v>1.2529962546816478</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1">
+        <v>1.4508230452674895</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="44">
         <v>5</v>
       </c>
       <c r="D6" s="19">
         <f t="shared" si="3"/>
-        <v>43111.374647887329</v>
+        <v>43110.861971830986</v>
       </c>
       <c r="E6" s="20">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F6" s="42" t="str">
+      <c r="F6" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="48" t="str">
+      <c r="H6" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="29" thickBot="1">
+    <row r="7" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="44">
         <v>6</v>
       </c>
       <c r="D7" s="19">
         <f t="shared" si="3"/>
-        <v>43115.083299798796</v>
+        <v>43114.367806841045</v>
       </c>
       <c r="E7" s="20">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F7" s="42" t="str">
+      <c r="F7" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H7" s="48" t="str">
+      <c r="H7" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="J7" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="K7" s="40">
+      <c r="K7" s="39">
         <f ca="1">+K4*1.5</f>
-        <v>20.026685393258425</v>
+        <v>22.782407407407408</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="M7" s="40">
+      <c r="M7" s="39">
         <f ca="1">+M4*1.5</f>
-        <v>13.156460674157302</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="29" thickBot="1">
+        <v>15.23364197530864</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="44">
         <v>6</v>
       </c>
       <c r="D8" s="19">
         <f t="shared" si="3"/>
-        <v>43118.791951710264</v>
+        <v>43117.873641851103</v>
       </c>
       <c r="E8" s="20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F8" s="42" t="str">
+      <c r="F8" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G8" s="60" t="s">
+      <c r="G8" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H8" s="48" t="str">
+      <c r="H8" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="J8" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="K8" s="40">
+      <c r="K8" s="39">
         <f ca="1">+K5*1.5</f>
-        <v>2.8609550561797752</v>
+        <v>3.2546296296296298</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="M8" s="40">
+      <c r="M8" s="39">
         <f ca="1">+M5*1.5</f>
-        <v>1.8794943820224717</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>2.1762345679012345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>3.2</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="44">
         <v>1</v>
       </c>
       <c r="D9" s="19">
         <f t="shared" si="3"/>
-        <v>43119.410060362177</v>
+        <v>43118.457947686111</v>
       </c>
       <c r="E9" s="20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F9" s="42" t="str">
+      <c r="F9" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="48" t="str">
+      <c r="H9" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>3.3</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="44">
         <f>2+(5/60)</f>
         <v>2.0833333333333335</v>
       </c>
       <c r="D10" s="19">
         <f t="shared" si="3"/>
-        <v>43120.697786720324</v>
+        <v>43119.675251509048</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F10" s="42" t="str">
+      <c r="F10" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G10" s="60" t="s">
+      <c r="G10" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H10" s="48" t="str">
+      <c r="H10" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="J10" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>3.4</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="53">
+      <c r="C11" s="52">
         <v>1</v>
       </c>
       <c r="D11" s="19">
         <f t="shared" si="3"/>
-        <v>43121.315895372238</v>
+        <v>43120.259557344056</v>
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F11" s="42" t="str">
+      <c r="F11" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G11" s="60" t="s">
+      <c r="G11" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H11" s="48" t="str">
+      <c r="H11" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J11" s="73" t="s">
+      <c r="J11" s="72" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C12" s="44">
         <v>6</v>
       </c>
       <c r="D12" s="19">
         <f t="shared" si="3"/>
-        <v>43125.024547283705</v>
+        <v>43123.765392354115</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F12" s="42" t="str">
+      <c r="F12" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G12" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="H12" s="48" t="str">
+        <v>DUE</v>
+      </c>
+      <c r="G12" s="59"/>
+      <c r="H12" s="47">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="J12" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="64"/>
-      <c r="N12" s="64"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="65"/>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="64"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="44">
         <v>6</v>
       </c>
       <c r="D13" s="19">
         <f t="shared" si="3"/>
-        <v>43128.733199195172</v>
+        <v>43127.271227364174</v>
       </c>
       <c r="E13" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F13" s="42" t="str">
+      <c r="F13" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>DUE</v>
       </c>
-      <c r="G13" s="60"/>
-      <c r="H13" s="48">
+      <c r="G13" s="59"/>
+      <c r="H13" s="47">
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
-      <c r="J13" s="66" t="s">
+      <c r="J13" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
-      <c r="O13" s="67"/>
-      <c r="P13" s="67"/>
-      <c r="Q13" s="68"/>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="67"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="44">
         <v>6</v>
       </c>
       <c r="D14" s="19">
         <f t="shared" si="3"/>
-        <v>43132.44185110664</v>
+        <v>43130.777062374233</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F14" s="42" t="str">
+      <c r="F14" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>DUE</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="48">
+      <c r="G14" s="59"/>
+      <c r="H14" s="47">
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
-      <c r="J14" s="69" t="s">
+      <c r="J14" s="68" t="s">
         <v>135</v>
       </c>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="67"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="67"/>
-      <c r="P14" s="67"/>
-      <c r="Q14" s="68"/>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="67"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="44">
         <v>6</v>
       </c>
       <c r="D15" s="19">
         <f t="shared" si="3"/>
-        <v>43136.150503018107</v>
+        <v>43134.282897384292</v>
       </c>
       <c r="E15" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F15" s="42" t="str">
+      <c r="F15" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>DUE</v>
       </c>
-      <c r="G15" s="60"/>
-      <c r="H15" s="48">
+      <c r="G15" s="59"/>
+      <c r="H15" s="47">
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
-      <c r="J15" s="70" t="s">
+      <c r="J15" s="69" t="s">
         <v>136</v>
       </c>
-      <c r="K15" s="71"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="71"/>
-      <c r="N15" s="71"/>
-      <c r="O15" s="71"/>
-      <c r="P15" s="71"/>
-      <c r="Q15" s="72"/>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="K15" s="70"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="70"/>
+      <c r="O15" s="70"/>
+      <c r="P15" s="70"/>
+      <c r="Q15" s="71"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="44">
         <v>6</v>
       </c>
       <c r="D16" s="19">
         <f t="shared" si="3"/>
-        <v>43139.859154929574</v>
+        <v>43137.788732394351</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F16" s="42" t="str">
+      <c r="F16" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>DUE</v>
       </c>
-      <c r="G16" s="60"/>
-      <c r="H16" s="48">
+      <c r="G16" s="59"/>
+      <c r="H16" s="47">
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="44">
         <v>5</v>
       </c>
       <c r="D17" s="19">
         <f t="shared" si="3"/>
-        <v>43142.949698189135</v>
+        <v>43140.710261569402</v>
       </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F17" s="42" t="str">
+      <c r="F17" s="41" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>DUE</v>
+      </c>
+      <c r="G17" s="59"/>
+      <c r="H17" s="47">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J17" s="73" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="44">
+        <v>3</v>
+      </c>
+      <c r="D18" s="19">
+        <f t="shared" si="3"/>
+        <v>43142.463179074432</v>
+      </c>
+      <c r="E18" s="20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F18" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>SOON</v>
       </c>
-      <c r="G17" s="60"/>
-      <c r="H17" s="48">
+      <c r="G18" s="59"/>
+      <c r="H18" s="47">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="J17" s="74" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="45">
         <v>3</v>
       </c>
-      <c r="D18" s="19">
-        <f t="shared" si="3"/>
-        <v>43144.804024144869</v>
-      </c>
-      <c r="E18" s="20">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="F18" s="42" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="48" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="44">
         <v>1.5</v>
       </c>
       <c r="D19" s="19">
         <f t="shared" si="3"/>
-        <v>43145.731187122736</v>
+        <v>43143.339637826946</v>
       </c>
       <c r="E19" s="20">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="F19" s="42" t="str">
+        <v>6</v>
+      </c>
+      <c r="F19" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G19" s="60"/>
-      <c r="H19" s="48" t="str">
+      <c r="G19" s="59"/>
+      <c r="H19" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="44">
         <v>6</v>
       </c>
       <c r="D20" s="19">
         <f t="shared" si="3"/>
-        <v>43149.439839034203</v>
+        <v>43146.845472837005</v>
       </c>
       <c r="E20" s="20">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F20" s="42" t="str">
+      <c r="F20" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G20" s="60"/>
-      <c r="H20" s="48" t="str">
+      <c r="G20" s="59"/>
+      <c r="H20" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="44">
         <v>4</v>
       </c>
       <c r="D21" s="19">
         <f t="shared" si="3"/>
-        <v>43151.91227364185</v>
+        <v>43149.182696177042</v>
       </c>
       <c r="E21" s="20">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="F21" s="42" t="str">
+        <v>7</v>
+      </c>
+      <c r="F21" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G21" s="60"/>
-      <c r="H21" s="48" t="str">
+      <c r="G21" s="59"/>
+      <c r="H21" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>65</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="44">
         <v>0.5</v>
       </c>
       <c r="D22" s="19">
         <f t="shared" si="3"/>
-        <v>43152.221327967804</v>
+        <v>43149.474849094549</v>
       </c>
       <c r="E22" s="20">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="F22" s="42" t="str">
+        <v>7</v>
+      </c>
+      <c r="F22" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G22" s="60"/>
-      <c r="H22" s="48" t="str">
+      <c r="G22" s="59"/>
+      <c r="H22" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="53">
+      <c r="C23" s="52">
         <v>3</v>
       </c>
       <c r="D23" s="19">
         <f t="shared" si="3"/>
-        <v>43154.075653923537</v>
+        <v>43151.227766599579</v>
       </c>
       <c r="E23" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F23" s="42" t="str">
+      <c r="F23" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G23" s="60"/>
-      <c r="H23" s="48" t="str">
+      <c r="G23" s="59"/>
+      <c r="H23" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="45">
+      <c r="C24" s="44">
         <v>2</v>
       </c>
       <c r="D24" s="19">
         <f t="shared" si="3"/>
-        <v>43155.311871227357</v>
+        <v>43152.396378269601</v>
       </c>
       <c r="E24" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F24" s="42" t="str">
+      <c r="F24" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G24" s="60"/>
-      <c r="H24" s="48" t="str">
+      <c r="G24" s="59"/>
+      <c r="H24" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="45">
+      <c r="C25" s="44">
         <v>2</v>
       </c>
       <c r="D25" s="19">
         <f t="shared" si="3"/>
-        <v>43156.548088531177</v>
+        <v>43153.564989939623</v>
       </c>
       <c r="E25" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F25" s="42" t="str">
+      <c r="F25" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G25" s="60"/>
-      <c r="H25" s="48" t="str">
+      <c r="G25" s="59"/>
+      <c r="H25" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="45">
+      <c r="C26" s="44">
         <v>2</v>
       </c>
       <c r="D26" s="19">
         <f t="shared" si="3"/>
-        <v>43157.784305834997</v>
+        <v>43154.733601609645</v>
       </c>
       <c r="E26" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F26" s="42" t="str">
+      <c r="F26" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G26" s="60"/>
-      <c r="H26" s="48" t="str">
+      <c r="G26" s="59"/>
+      <c r="H26" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>5.2</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="53">
+      <c r="C27" s="52">
         <v>10</v>
       </c>
       <c r="D27" s="19">
         <f t="shared" si="3"/>
-        <v>43163.965392354112</v>
+        <v>43160.576659959748</v>
       </c>
       <c r="E27" s="20">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F27" s="42" t="str">
+      <c r="F27" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G27" s="60"/>
-      <c r="H27" s="48" t="str">
+      <c r="G27" s="59"/>
+      <c r="H27" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C28" s="44">
         <v>5</v>
       </c>
       <c r="D28" s="19">
         <f t="shared" si="3"/>
-        <v>43167.055935613673</v>
+        <v>43163.4981891348</v>
       </c>
       <c r="E28" s="20">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F28" s="42" t="str">
+        <v>9</v>
+      </c>
+      <c r="F28" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G28" s="60"/>
-      <c r="H28" s="48" t="str">
+      <c r="G28" s="59"/>
+      <c r="H28" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C29" s="45">
         <v>6</v>
       </c>
       <c r="D29" s="19">
         <f t="shared" si="3"/>
-        <v>43170.76458752514</v>
+        <v>43167.004024144859</v>
       </c>
       <c r="E29" s="20">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F29" s="42" t="str">
+      <c r="F29" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G29" s="60"/>
-      <c r="H29" s="48" t="str">
+      <c r="G29" s="59"/>
+      <c r="H29" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J29" s="57" t="s">
+      <c r="J29" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K29" s="57"/>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="K29" s="56"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="46">
+      <c r="C30" s="45">
         <v>1.5</v>
       </c>
       <c r="D30" s="19">
         <f t="shared" si="3"/>
-        <v>43171.691750503007</v>
+        <v>43167.880482897373</v>
       </c>
       <c r="E30" s="20">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F30" s="42" t="str">
+      <c r="F30" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G30" s="60"/>
-      <c r="H30" s="48" t="str">
+      <c r="G30" s="59"/>
+      <c r="H30" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J30" s="57" t="s">
+      <c r="J30" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K30" s="57"/>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="K30" s="56"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="46">
+      <c r="C31" s="45">
         <v>1</v>
       </c>
       <c r="D31" s="19">
         <f t="shared" si="3"/>
-        <v>43172.309859154921</v>
+        <v>43168.464788732381</v>
       </c>
       <c r="E31" s="20">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="F31" s="42" t="str">
+        <v>10</v>
+      </c>
+      <c r="F31" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G31" s="60"/>
-      <c r="H31" s="48" t="str">
+      <c r="G31" s="59"/>
+      <c r="H31" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J31" s="57" t="s">
+      <c r="J31" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K31" s="57"/>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="K31" s="56"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="46">
+      <c r="C32" s="45">
         <v>2</v>
       </c>
       <c r="D32" s="19">
         <f t="shared" si="3"/>
-        <v>43173.546076458741</v>
+        <v>43169.633400402403</v>
       </c>
       <c r="E32" s="20">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="F32" s="42" t="str">
+        <v>10</v>
+      </c>
+      <c r="F32" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G32" s="60"/>
-      <c r="H32" s="48" t="str">
+      <c r="G32" s="59"/>
+      <c r="H32" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J32" s="57" t="s">
+      <c r="J32" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K32" s="57"/>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="K32" s="56"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>6.3</v>
       </c>
-      <c r="B33" s="56" t="s">
+      <c r="B33" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="46">
+      <c r="C33" s="45">
         <f>15/60</f>
         <v>0.25</v>
       </c>
       <c r="D33" s="19">
         <f t="shared" si="3"/>
-        <v>43173.700603621721</v>
+        <v>43169.779476861157</v>
       </c>
       <c r="E33" s="20">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="F33" s="42" t="str">
+        <v>10</v>
+      </c>
+      <c r="F33" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G33" s="60"/>
-      <c r="H33" s="48" t="str">
+      <c r="G33" s="59"/>
+      <c r="H33" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J33" s="57" t="s">
+      <c r="J33" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K33" s="57"/>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="K33" s="56"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>6.4</v>
       </c>
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="53">
+      <c r="C34" s="52">
         <v>6</v>
       </c>
       <c r="D34" s="19">
         <f t="shared" si="3"/>
-        <v>43177.409255533188</v>
+        <v>43173.285311871216</v>
       </c>
       <c r="E34" s="20">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="F34" s="42" t="str">
+      <c r="F34" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G34" s="60"/>
-      <c r="H34" s="48" t="str">
+      <c r="G34" s="59"/>
+      <c r="H34" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>7</v>
       </c>
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="53">
+      <c r="C35" s="52">
         <v>10</v>
       </c>
       <c r="D35" s="19">
         <f t="shared" si="3"/>
-        <v>43183.590342052303</v>
+        <v>43179.128370221319</v>
       </c>
       <c r="E35" s="20">
         <f t="shared" ref="E35:E54" si="4">ROUNDDOWN((D35-$M$1)/7, 0)+1</f>
         <v>12</v>
       </c>
-      <c r="F35" s="42" t="str">
+      <c r="F35" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G35" s="60"/>
-      <c r="H35" s="48" t="str">
+      <c r="G35" s="59"/>
+      <c r="H35" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="46">
+      <c r="C36" s="45">
         <v>3</v>
       </c>
       <c r="D36" s="19">
         <f t="shared" si="3"/>
-        <v>43185.444668008036</v>
+        <v>43180.881287726348</v>
       </c>
       <c r="E36" s="20">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="F36" s="42" t="str">
+      <c r="F36" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G36" s="60"/>
-      <c r="H36" s="48" t="str">
+      <c r="G36" s="59"/>
+      <c r="H36" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J36" s="57" t="s">
+      <c r="J36" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K36" s="57"/>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="K36" s="56"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="56" t="s">
+      <c r="B37" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="46">
+      <c r="C37" s="45">
         <v>3</v>
       </c>
       <c r="D37" s="19">
         <f t="shared" si="3"/>
-        <v>43187.29899396377</v>
+        <v>43182.634205231378</v>
       </c>
       <c r="E37" s="20">
         <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="F37" s="42" t="str">
+        <v>12</v>
+      </c>
+      <c r="F37" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G37" s="60"/>
-      <c r="H37" s="48" t="str">
+      <c r="G37" s="59"/>
+      <c r="H37" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J37" s="57" t="s">
+      <c r="J37" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K37" s="57"/>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="K37" s="56"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="46">
+      <c r="C38" s="45">
         <v>3</v>
       </c>
       <c r="D38" s="19">
         <f t="shared" si="3"/>
-        <v>43189.153319919504</v>
+        <v>43184.387122736407</v>
       </c>
       <c r="E38" s="20">
         <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="F38" s="42" t="str">
+        <v>12</v>
+      </c>
+      <c r="F38" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G38" s="60"/>
-      <c r="H38" s="48" t="str">
+      <c r="G38" s="59"/>
+      <c r="H38" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J38" s="57" t="s">
+      <c r="J38" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K38" s="57"/>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="K38" s="56"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="56" t="s">
+      <c r="B39" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="46">
+      <c r="C39" s="45">
         <v>6</v>
       </c>
       <c r="D39" s="19">
         <f t="shared" si="3"/>
-        <v>43192.861971830971</v>
+        <v>43187.892957746466</v>
       </c>
       <c r="E39" s="20">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="F39" s="42" t="str">
+      <c r="F39" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G39" s="60"/>
-      <c r="H39" s="48" t="str">
+      <c r="G39" s="59"/>
+      <c r="H39" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J39" s="57" t="s">
+      <c r="J39" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K39" s="57"/>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="K39" s="56"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="46">
+      <c r="C40" s="45">
         <v>3</v>
       </c>
       <c r="D40" s="19">
         <f t="shared" si="3"/>
-        <v>43194.716297786705</v>
+        <v>43189.645875251495</v>
       </c>
       <c r="E40" s="20">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="F40" s="42" t="str">
+        <v>13</v>
+      </c>
+      <c r="F40" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G40" s="60"/>
-      <c r="H40" s="48" t="str">
+      <c r="G40" s="59"/>
+      <c r="H40" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J40" s="57" t="s">
+      <c r="J40" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K40" s="57"/>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="K40" s="56"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="46">
+      <c r="C41" s="45">
         <v>2</v>
       </c>
       <c r="D41" s="19">
         <f t="shared" si="3"/>
-        <v>43195.952515090525</v>
+        <v>43190.814486921518</v>
       </c>
       <c r="E41" s="20">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="F41" s="42" t="str">
+        <v>13</v>
+      </c>
+      <c r="F41" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G41" s="60"/>
-      <c r="H41" s="48" t="str">
+      <c r="G41" s="59"/>
+      <c r="H41" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J41" s="57" t="s">
+      <c r="J41" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K41" s="57"/>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="K41" s="56"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="56" t="s">
+      <c r="B42" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="46">
+      <c r="C42" s="45">
         <v>3</v>
       </c>
       <c r="D42" s="19">
         <f t="shared" si="3"/>
-        <v>43197.806841046258</v>
+        <v>43192.567404426547</v>
       </c>
       <c r="E42" s="20">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="F42" s="42" t="str">
+        <v>13</v>
+      </c>
+      <c r="F42" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G42" s="60"/>
-      <c r="H42" s="48" t="str">
+      <c r="G42" s="59"/>
+      <c r="H42" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J42" s="57" t="s">
+      <c r="J42" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K42" s="57"/>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="K42" s="56"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="46">
+      <c r="C43" s="45">
         <v>3</v>
       </c>
       <c r="D43" s="19">
         <f t="shared" si="3"/>
-        <v>43199.661167001992</v>
+        <v>43194.320321931576</v>
       </c>
       <c r="E43" s="20">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="F43" s="42" t="str">
+      <c r="F43" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G43" s="60"/>
-      <c r="H43" s="48" t="str">
+      <c r="G43" s="59"/>
+      <c r="H43" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J43" s="57" t="s">
+      <c r="J43" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K43" s="57"/>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="K43" s="56"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="46">
+      <c r="C44" s="45">
         <v>3</v>
       </c>
       <c r="D44" s="19">
         <f t="shared" si="3"/>
-        <v>43201.515492957726</v>
+        <v>43196.073239436606</v>
       </c>
       <c r="E44" s="20">
         <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="F44" s="42" t="str">
+        <v>14</v>
+      </c>
+      <c r="F44" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G44" s="60"/>
-      <c r="H44" s="48" t="str">
+      <c r="G44" s="59"/>
+      <c r="H44" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J44" s="57" t="s">
+      <c r="J44" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K44" s="57"/>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="K44" s="56"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="56" t="s">
+      <c r="B45" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="46">
+      <c r="C45" s="45">
         <v>2</v>
       </c>
       <c r="D45" s="19">
         <f t="shared" si="3"/>
-        <v>43202.751710261546</v>
+        <v>43197.241851106628</v>
       </c>
       <c r="E45" s="20">
         <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="F45" s="42" t="str">
+        <v>14</v>
+      </c>
+      <c r="F45" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G45" s="60"/>
-      <c r="H45" s="48" t="str">
+      <c r="G45" s="59"/>
+      <c r="H45" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J45" s="57" t="s">
+      <c r="J45" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K45" s="57"/>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="K45" s="56"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>8.4</v>
       </c>
-      <c r="B46" s="56" t="s">
+      <c r="B46" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="46">
+      <c r="C46" s="45">
         <v>3</v>
       </c>
       <c r="D46" s="19">
         <f t="shared" si="3"/>
-        <v>43204.606036217279</v>
+        <v>43198.994768611657</v>
       </c>
       <c r="E46" s="20">
         <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="F46" s="42" t="str">
+        <v>14</v>
+      </c>
+      <c r="F46" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G46" s="60"/>
-      <c r="H46" s="48" t="str">
+      <c r="G46" s="59"/>
+      <c r="H46" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J46" s="57" t="s">
+      <c r="J46" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K46" s="57"/>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="K46" s="56"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="46">
+      <c r="C47" s="45">
         <v>3</v>
       </c>
       <c r="D47" s="19">
         <f t="shared" si="3"/>
-        <v>43206.460362173013</v>
+        <v>43200.747686116687</v>
       </c>
       <c r="E47" s="20">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="F47" s="42" t="str">
+      <c r="F47" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G47" s="60"/>
-      <c r="H47" s="48" t="str">
+      <c r="G47" s="59"/>
+      <c r="H47" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J47" s="57" t="s">
+      <c r="J47" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K47" s="57"/>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="K47" s="56"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="46">
+      <c r="C48" s="45">
         <v>6</v>
       </c>
       <c r="D48" s="19">
         <f t="shared" si="3"/>
-        <v>43210.16901408448</v>
+        <v>43204.253521126746</v>
       </c>
       <c r="E48" s="20">
         <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="F48" s="42" t="str">
+        <v>15</v>
+      </c>
+      <c r="F48" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G48" s="60"/>
-      <c r="H48" s="48" t="str">
+      <c r="G48" s="59"/>
+      <c r="H48" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J48" s="57" t="s">
+      <c r="J48" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K48" s="57"/>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="K48" s="56"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="46">
+      <c r="C49" s="45">
         <v>2</v>
       </c>
       <c r="D49" s="19">
         <f t="shared" si="3"/>
-        <v>43211.4052313883</v>
+        <v>43205.422132796768</v>
       </c>
       <c r="E49" s="20">
         <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="F49" s="42" t="str">
+        <v>15</v>
+      </c>
+      <c r="F49" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G49" s="60"/>
-      <c r="H49" s="48" t="str">
+      <c r="G49" s="59"/>
+      <c r="H49" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J49" s="57" t="s">
+      <c r="J49" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="K49" s="57"/>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="K49" s="56"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>9.1</v>
       </c>
-      <c r="B50" s="54" t="s">
+      <c r="B50" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="53">
+      <c r="C50" s="52">
         <f>30/5</f>
         <v>6</v>
       </c>
       <c r="D50" s="19">
         <f t="shared" si="3"/>
-        <v>43215.113883299768</v>
+        <v>43208.927967806827</v>
       </c>
       <c r="E50" s="20">
         <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-      <c r="F50" s="42" t="str">
+        <v>16</v>
+      </c>
+      <c r="F50" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G50" s="60"/>
-      <c r="H50" s="48" t="str">
+      <c r="G50" s="59"/>
+      <c r="H50" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B51" s="54" t="s">
+      <c r="B51" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="C51" s="53">
+      <c r="C51" s="52">
         <f>30/5</f>
         <v>6</v>
       </c>
       <c r="D51" s="19">
         <f t="shared" si="3"/>
-        <v>43218.822535211235</v>
+        <v>43212.433802816886</v>
       </c>
       <c r="E51" s="20">
         <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-      <c r="F51" s="42" t="str">
+        <v>16</v>
+      </c>
+      <c r="F51" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G51" s="60"/>
-      <c r="H51" s="48" t="str">
+      <c r="G51" s="59"/>
+      <c r="H51" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B52" s="54" t="s">
+      <c r="B52" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="53">
+      <c r="C52" s="52">
         <f>30/5</f>
         <v>6</v>
       </c>
       <c r="D52" s="19">
         <f t="shared" si="3"/>
-        <v>43222.531187122702</v>
+        <v>43215.939637826945</v>
       </c>
       <c r="E52" s="20">
         <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="F52" s="42" t="str">
+        <v>17</v>
+      </c>
+      <c r="F52" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G52" s="60"/>
-      <c r="H52" s="48" t="str">
+      <c r="G52" s="59"/>
+      <c r="H52" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>9.4</v>
       </c>
-      <c r="B53" s="54" t="s">
+      <c r="B53" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="53">
+      <c r="C53" s="52">
         <f>30/5</f>
         <v>6</v>
       </c>
       <c r="D53" s="19">
         <f t="shared" si="3"/>
-        <v>43226.23983903417</v>
+        <v>43219.445472837004</v>
       </c>
       <c r="E53" s="20">
         <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="F53" s="42" t="str">
+        <v>17</v>
+      </c>
+      <c r="F53" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G53" s="60"/>
-      <c r="H53" s="48" t="str">
+      <c r="G53" s="59"/>
+      <c r="H53" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>9.5</v>
       </c>
-      <c r="B54" s="54" t="s">
+      <c r="B54" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="C54" s="53">
+      <c r="C54" s="52">
         <f>30/5</f>
         <v>6</v>
       </c>
       <c r="D54" s="19">
         <f t="shared" si="3"/>
-        <v>43229.948490945637</v>
+        <v>43222.951307847063</v>
       </c>
       <c r="E54" s="20">
         <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="F54" s="42" t="str">
+        <v>18</v>
+      </c>
+      <c r="F54" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G54" s="60"/>
-      <c r="H54" s="48" t="str">
+      <c r="G54" s="59"/>
+      <c r="H54" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1">
-      <c r="B56" s="50" t="s">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="47">
+      <c r="C56" s="46">
         <f>SUM(C1:C55)</f>
         <v>207.08333333333331</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15" thickTop="1">
-      <c r="B57" s="50"/>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="B58" s="50" t="s">
+    <row r="57" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="49"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="C58" s="51">
+      <c r="C58" s="50">
         <f>C56-C59</f>
-        <v>37.333333333333314</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="B59" s="50" t="s">
+        <v>31.333333333333314</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="C59" s="51">
+      <c r="C59" s="50">
         <f>SUMIF(G2:G54, "", C2:C54)</f>
-        <v>169.75</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="B62" s="55" t="s">
+        <v>175.75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="C62" s="53">
+      <c r="C62" s="52">
         <f>SUM(C50:C54,C34:C35, C27, C23, C11, C4)</f>
         <v>61.5</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
-      <c r="B63" s="52" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="C63" s="45">
+      <c r="C63" s="44">
         <f>C56-C62</f>
         <v>145.58333333333331</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
-      <c r="B64" s="52" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="45">
+      <c r="C64" s="44">
         <f>C63*0.6</f>
         <v>87.34999999999998</v>
       </c>
     </row>
-    <row r="66" spans="2:3" ht="15" thickBot="1">
-      <c r="B66" s="50" t="s">
+    <row r="66" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="C66" s="47">
+      <c r="C66" s="46">
         <f>C62+C64</f>
         <v>148.84999999999997</v>
       </c>
     </row>
-    <row r="67" spans="2:3" ht="15" thickTop="1">
-      <c r="B67" s="50"/>
-    </row>
-    <row r="68" spans="2:3">
-      <c r="B68" s="50" t="s">
+    <row r="67" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="49"/>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="C68" s="51">
+      <c r="C68" s="50">
         <f>C58</f>
-        <v>37.333333333333314</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3">
-      <c r="B69" s="50" t="s">
+        <v>31.333333333333314</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="C69" s="51">
+      <c r="C69" s="50">
         <f>C66-C68</f>
-        <v>111.51666666666665</v>
+        <v>117.51666666666665</v>
       </c>
     </row>
   </sheetData>
@@ -3492,33 +3518,33 @@
   <dimension ref="A1:R57"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.6640625" style="36" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.83203125" customWidth="1"/>
-    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.7109375" style="36" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="46" thickBot="1">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>2</v>
       </c>
@@ -3568,7 +3594,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -3595,7 +3621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2.1</v>
       </c>
@@ -3624,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>2.2000000000000002</v>
       </c>
@@ -3652,7 +3678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
@@ -3680,7 +3706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -3708,7 +3734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
@@ -3736,7 +3762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -3764,7 +3790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>3.2</v>
       </c>
@@ -3792,7 +3818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>3.3</v>
       </c>
@@ -3821,7 +3847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>3.4</v>
       </c>
@@ -3849,7 +3875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
@@ -3877,7 +3903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
@@ -3905,7 +3931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -3933,7 +3959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>27</v>
       </c>
@@ -3961,7 +3987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>58</v>
       </c>
@@ -3989,7 +4015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>59</v>
       </c>
@@ -4017,7 +4043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>60</v>
       </c>
@@ -4045,7 +4071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>61</v>
       </c>
@@ -4073,7 +4099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
@@ -4101,7 +4127,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>64</v>
       </c>
@@ -4129,7 +4155,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>65</v>
       </c>
@@ -4157,7 +4183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>67</v>
       </c>
@@ -4185,7 +4211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>69</v>
       </c>
@@ -4213,7 +4239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>70</v>
       </c>
@@ -4241,7 +4267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>71</v>
       </c>
@@ -4269,7 +4295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>5.2</v>
       </c>
@@ -4297,7 +4323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>72</v>
       </c>
@@ -4325,7 +4351,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>73</v>
       </c>
@@ -4353,7 +4379,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>74</v>
       </c>
@@ -4381,7 +4407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>75</v>
       </c>
@@ -4409,7 +4435,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>76</v>
       </c>
@@ -4437,7 +4463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>6.3</v>
       </c>
@@ -4466,7 +4492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>6.4</v>
       </c>
@@ -4494,7 +4520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>7</v>
       </c>
@@ -4522,7 +4548,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
@@ -4550,7 +4576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>80</v>
       </c>
@@ -4578,7 +4604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>81</v>
       </c>
@@ -4606,7 +4632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>83</v>
       </c>
@@ -4634,7 +4660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>84</v>
       </c>
@@ -4662,7 +4688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>86</v>
       </c>
@@ -4690,7 +4716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>88</v>
       </c>
@@ -4718,7 +4744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>89</v>
       </c>
@@ -4746,7 +4772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>90</v>
       </c>
@@ -4774,7 +4800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>91</v>
       </c>
@@ -4802,7 +4828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>8.4</v>
       </c>
@@ -4830,7 +4856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>93</v>
       </c>
@@ -4858,7 +4884,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>94</v>
       </c>
@@ -4886,7 +4912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>95</v>
       </c>
@@ -4914,7 +4940,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>9.1</v>
       </c>
@@ -4943,7 +4969,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>9.1999999999999993</v>
       </c>
@@ -4972,7 +4998,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>9.3000000000000007</v>
       </c>
@@ -5001,7 +5027,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>9.4</v>
       </c>
@@ -5030,7 +5056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>9.5</v>
       </c>
@@ -5059,13 +5085,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15" thickBot="1">
-      <c r="C56" s="39">
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="38">
         <f>SUM(C1:C55)</f>
         <v>207.08333333333331</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15" thickTop="1"/>
+    <row r="57" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
@@ -5086,24 +5112,24 @@
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="15:16">
+    <row r="1" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O1" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="15:16">
+    <row r="2" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O2" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="15:16">
+    <row r="3" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O3" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="15:16">
+    <row r="4" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O4" s="4">
         <v>43132</v>
       </c>

</xml_diff>

<commit_message>
Finished ch 2 of 4 - pandas Foundations - DataCamp
</commit_message>
<xml_diff>
--- a/Springboard Course Schedule & Study Plan.xlsx
+++ b/Springboard Course Schedule & Study Plan.xlsx
@@ -883,7 +883,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1070,6 +1070,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="31">
@@ -1639,7 +1642,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C2:C9"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1714,7 @@
       <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="77" t="s">
         <v>68</v>
       </c>
       <c r="C2" s="43">

</xml_diff>

<commit_message>
Finished ch 4 of 4 - pandas Foundations - DataCamp and got certificate
</commit_message>
<xml_diff>
--- a/Springboard Course Schedule & Study Plan.xlsx
+++ b/Springboard Course Schedule & Study Plan.xlsx
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="139">
   <si>
     <t>Description</t>
   </si>
@@ -554,7 +554,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,6 +626,14 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1068,11 +1076,11 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="31">
@@ -1642,7 +1650,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12:H18"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,7 +1722,7 @@
       <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="76" t="s">
         <v>68</v>
       </c>
       <c r="C2" s="43">
@@ -1818,14 +1826,14 @@
       </c>
       <c r="K4" s="39">
         <f ca="1">K5*7</f>
-        <v>15.188271604938272</v>
+        <v>14.853125000000002</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>123</v>
       </c>
       <c r="M4" s="39">
         <f ca="1">M5*7</f>
-        <v>10.155761316872427</v>
+        <v>9.7577083333333317</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1862,14 +1870,14 @@
       </c>
       <c r="K5" s="39">
         <f ca="1">C59/(M2-TODAY())</f>
-        <v>2.1697530864197532</v>
+        <v>2.1218750000000002</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>124</v>
       </c>
       <c r="M5" s="39">
         <f ca="1">C69/(M2-TODAY())</f>
-        <v>1.4508230452674895</v>
+        <v>1.3939583333333332</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1936,14 +1944,14 @@
       </c>
       <c r="K7" s="39">
         <f ca="1">+K4*1.5</f>
-        <v>22.782407407407408</v>
+        <v>22.279687500000001</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>130</v>
       </c>
       <c r="M7" s="39">
         <f ca="1">+M4*1.5</f>
-        <v>15.23364197530864</v>
+        <v>14.636562499999997</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1980,14 +1988,14 @@
       </c>
       <c r="K8" s="39">
         <f ca="1">+K5*1.5</f>
-        <v>3.2546296296296298</v>
+        <v>3.1828125000000003</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>131</v>
       </c>
       <c r="M8" s="39">
         <f ca="1">+M5*1.5</f>
-        <v>2.1762345679012345</v>
+        <v>2.0909374999999999</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2050,7 +2058,7 @@
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J10" s="76" t="s">
+      <c r="J10" s="77" t="s">
         <v>138</v>
       </c>
       <c r="K10" s="14"/>
@@ -2108,12 +2116,14 @@
       </c>
       <c r="F12" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DUE</v>
-      </c>
-      <c r="G12" s="59"/>
-      <c r="H12" s="47">
+        <v/>
+      </c>
+      <c r="G12" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v/>
       </c>
       <c r="J12" s="62" t="s">
         <v>133</v>
@@ -3435,7 +3445,7 @@
       </c>
       <c r="C58" s="50">
         <f>C56-C59</f>
-        <v>31.333333333333314</v>
+        <v>37.333333333333314</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3444,7 +3454,7 @@
       </c>
       <c r="C59" s="50">
         <f>SUMIF(G2:G54, "", C2:C54)</f>
-        <v>175.75</v>
+        <v>169.75</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3492,7 +3502,7 @@
       </c>
       <c r="C68" s="50">
         <f>C58</f>
-        <v>31.333333333333314</v>
+        <v>37.333333333333314</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -3501,13 +3511,13 @@
       </c>
       <c r="C69" s="50">
         <f>C66-C68</f>
-        <v>117.51666666666665</v>
+        <v>111.51666666666665</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
progress on ch 1 of 5 - Manipulating DataFrames with pandas - DataCamp
</commit_message>
<xml_diff>
--- a/Springboard Course Schedule & Study Plan.xlsx
+++ b/Springboard Course Schedule & Study Plan.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Improved Dynamic Study Plan" sheetId="4" r:id="rId1"/>
-    <sheet name="Dynamic Springboard Study Plan" sheetId="1" r:id="rId2"/>
-    <sheet name="Springboard Study Plan" sheetId="2" r:id="rId3"/>
+    <sheet name="Ref - Springboard plan in Excel" sheetId="1" r:id="rId2"/>
+    <sheet name="Ref - Springboard Study Plan" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="140">
   <si>
     <t>Description</t>
   </si>
@@ -483,12 +483,6 @@
     <t>Target End Date:</t>
   </si>
   <si>
-    <t>Capstone Project Hours</t>
-  </si>
-  <si>
-    <t>Curriculum Hours</t>
-  </si>
-  <si>
     <t>TOTAL HOURS FOR CERT</t>
   </si>
   <si>
@@ -544,15 +538,25 @@
   </si>
   <si>
     <t>Customize by changing blue cells</t>
+  </si>
+  <si>
+    <t>Total Capstone Project Hours</t>
+  </si>
+  <si>
+    <t>Total Curriculum Hours</t>
+  </si>
+  <si>
+    <t>Capstone Hours Required for Cert (100%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -633,7 +637,7 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="9.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -858,7 +862,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -890,8 +894,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1079,11 +1084,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="32">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1115,6 +1123,7 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="31" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1646,11 +1655,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q69"/>
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,7 +1679,7 @@
     <col min="10" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="5.7109375" customWidth="1"/>
     <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2.7109375" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
     <col min="16" max="16" width="5.85546875" customWidth="1"/>
@@ -1702,7 +1714,7 @@
       </c>
       <c r="K1" s="74">
         <f>K2*7</f>
-        <v>11.980027548209366</v>
+        <v>11.324869791666666</v>
       </c>
       <c r="L1" s="15" t="s">
         <v>7</v>
@@ -1711,11 +1723,11 @@
         <v>43102</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P1" s="57">
         <f>ROUND((M2-M1+1)/30, 2)</f>
-        <v>4.03</v>
+        <v>4.2699999999999996</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1752,13 +1764,13 @@
       </c>
       <c r="K2" s="39">
         <f>C56/(M2-M1+1)</f>
-        <v>1.7114325068870522</v>
+        <v>1.6178385416666665</v>
       </c>
       <c r="L2" s="37" t="s">
         <v>117</v>
       </c>
       <c r="M2" s="75">
-        <v>43222</v>
+        <v>43229</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1774,7 +1786,7 @@
       </c>
       <c r="D3" s="19">
         <f>D2+$C3/K$2</f>
-        <v>43102.389537223338</v>
+        <v>43102.412072434607</v>
       </c>
       <c r="E3" s="20">
         <f t="shared" ref="E3:E34" si="0">ROUNDDOWN((D3-$M$1)/7, 0)+1</f>
@@ -1804,7 +1816,7 @@
       </c>
       <c r="D4" s="19">
         <f t="shared" ref="D4:D54" si="3">D3+$C4/K$2</f>
-        <v>43103.265995975853</v>
+        <v>43103.339235412473</v>
       </c>
       <c r="E4" s="20">
         <f t="shared" si="0"/>
@@ -1826,14 +1838,14 @@
       </c>
       <c r="K4" s="39">
         <f ca="1">K5*7</f>
-        <v>14.853125000000002</v>
+        <v>13.658045977011493</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M4" s="39">
         <f ca="1">M5*7</f>
-        <v>9.7577083333333317</v>
+        <v>8.9726053639846732</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1848,7 +1860,7 @@
       </c>
       <c r="D5" s="19">
         <f t="shared" si="3"/>
-        <v>43107.940442655934</v>
+        <v>43108.284104627768</v>
       </c>
       <c r="E5" s="20">
         <f t="shared" si="0"/>
@@ -1869,15 +1881,15 @@
         <v>115</v>
       </c>
       <c r="K5" s="39">
-        <f ca="1">C59/(M2-TODAY())</f>
-        <v>2.1218750000000002</v>
+        <f ca="1">C62/(M2-TODAY())</f>
+        <v>1.9511494252873562</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M5" s="39">
-        <f ca="1">C69/(M2-TODAY())</f>
-        <v>1.3939583333333332</v>
+        <f ca="1">C71/(M2-TODAY())</f>
+        <v>1.2818007662835247</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1892,7 +1904,7 @@
       </c>
       <c r="D6" s="19">
         <f t="shared" si="3"/>
-        <v>43110.861971830986</v>
+        <v>43111.374647887329</v>
       </c>
       <c r="E6" s="20">
         <f t="shared" si="0"/>
@@ -1922,7 +1934,7 @@
       </c>
       <c r="D7" s="19">
         <f t="shared" si="3"/>
-        <v>43114.367806841045</v>
+        <v>43115.083299798796</v>
       </c>
       <c r="E7" s="20">
         <f t="shared" si="0"/>
@@ -1940,18 +1952,18 @@
         <v/>
       </c>
       <c r="J7" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K7" s="39">
         <f ca="1">+K4*1.5</f>
-        <v>22.279687500000001</v>
+        <v>20.487068965517238</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M7" s="39">
         <f ca="1">+M4*1.5</f>
-        <v>14.636562499999997</v>
+        <v>13.45890804597701</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1966,7 +1978,7 @@
       </c>
       <c r="D8" s="19">
         <f t="shared" si="3"/>
-        <v>43117.873641851103</v>
+        <v>43118.791951710264</v>
       </c>
       <c r="E8" s="20">
         <f t="shared" si="0"/>
@@ -1984,18 +1996,18 @@
         <v/>
       </c>
       <c r="J8" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K8" s="39">
         <f ca="1">+K5*1.5</f>
-        <v>3.1828125000000003</v>
+        <v>2.9267241379310343</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M8" s="39">
         <f ca="1">+M5*1.5</f>
-        <v>2.0909374999999999</v>
+        <v>1.922701149425287</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2010,7 +2022,7 @@
       </c>
       <c r="D9" s="19">
         <f t="shared" si="3"/>
-        <v>43118.457947686111</v>
+        <v>43119.410060362177</v>
       </c>
       <c r="E9" s="20">
         <f t="shared" si="0"/>
@@ -2041,7 +2053,7 @@
       </c>
       <c r="D10" s="19">
         <f t="shared" si="3"/>
-        <v>43119.675251509048</v>
+        <v>43120.697786720324</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" si="0"/>
@@ -2058,8 +2070,8 @@
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J10" s="77" t="s">
-        <v>138</v>
+      <c r="J10" s="78" t="s">
+        <v>136</v>
       </c>
       <c r="K10" s="14"/>
     </row>
@@ -2075,7 +2087,7 @@
       </c>
       <c r="D11" s="19">
         <f t="shared" si="3"/>
-        <v>43120.259557344056</v>
+        <v>43121.315895372238</v>
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
@@ -2093,7 +2105,7 @@
         <v/>
       </c>
       <c r="J11" s="72" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -2108,7 +2120,7 @@
       </c>
       <c r="D12" s="19">
         <f t="shared" si="3"/>
-        <v>43123.765392354115</v>
+        <v>43125.024547283705</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
@@ -2126,7 +2138,7 @@
         <v/>
       </c>
       <c r="J12" s="62" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K12" s="63"/>
       <c r="L12" s="63"/>
@@ -2148,7 +2160,7 @@
       </c>
       <c r="D13" s="19">
         <f t="shared" si="3"/>
-        <v>43127.271227364174</v>
+        <v>43128.733199195172</v>
       </c>
       <c r="E13" s="20">
         <f t="shared" si="0"/>
@@ -2164,7 +2176,7 @@
         <v>6</v>
       </c>
       <c r="J13" s="65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K13" s="66"/>
       <c r="L13" s="66"/>
@@ -2186,7 +2198,7 @@
       </c>
       <c r="D14" s="19">
         <f t="shared" si="3"/>
-        <v>43130.777062374233</v>
+        <v>43132.44185110664</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
@@ -2202,7 +2214,7 @@
         <v>6</v>
       </c>
       <c r="J14" s="68" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K14" s="66"/>
       <c r="L14" s="66"/>
@@ -2224,7 +2236,7 @@
       </c>
       <c r="D15" s="19">
         <f t="shared" si="3"/>
-        <v>43134.282897384292</v>
+        <v>43136.150503018107</v>
       </c>
       <c r="E15" s="20">
         <f t="shared" si="0"/>
@@ -2240,7 +2252,7 @@
         <v>6</v>
       </c>
       <c r="J15" s="69" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K15" s="70"/>
       <c r="L15" s="70"/>
@@ -2262,7 +2274,7 @@
       </c>
       <c r="D16" s="19">
         <f t="shared" si="3"/>
-        <v>43137.788732394351</v>
+        <v>43139.859154929574</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
@@ -2290,7 +2302,7 @@
       </c>
       <c r="D17" s="19">
         <f t="shared" si="3"/>
-        <v>43140.710261569402</v>
+        <v>43142.949698189135</v>
       </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
@@ -2298,7 +2310,7 @@
       </c>
       <c r="F17" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DUE</v>
+        <v>SOON</v>
       </c>
       <c r="G17" s="59"/>
       <c r="H17" s="47">
@@ -2306,7 +2318,7 @@
         <v>5</v>
       </c>
       <c r="J17" s="73" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2321,20 +2333,20 @@
       </c>
       <c r="D18" s="19">
         <f t="shared" si="3"/>
-        <v>43142.463179074432</v>
+        <v>43144.804024144869</v>
       </c>
       <c r="E18" s="20">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F18" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SOON</v>
+        <v/>
       </c>
       <c r="G18" s="59"/>
-      <c r="H18" s="47">
+      <c r="H18" s="47" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2349,11 +2361,11 @@
       </c>
       <c r="D19" s="19">
         <f t="shared" si="3"/>
-        <v>43143.339637826946</v>
+        <v>43145.731187122736</v>
       </c>
       <c r="E19" s="20">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F19" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2377,7 +2389,7 @@
       </c>
       <c r="D20" s="19">
         <f t="shared" si="3"/>
-        <v>43146.845472837005</v>
+        <v>43149.439839034203</v>
       </c>
       <c r="E20" s="20">
         <f t="shared" si="0"/>
@@ -2405,11 +2417,11 @@
       </c>
       <c r="D21" s="19">
         <f t="shared" si="3"/>
-        <v>43149.182696177042</v>
+        <v>43151.91227364185</v>
       </c>
       <c r="E21" s="20">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F21" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2433,11 +2445,11 @@
       </c>
       <c r="D22" s="19">
         <f t="shared" si="3"/>
-        <v>43149.474849094549</v>
+        <v>43152.221327967804</v>
       </c>
       <c r="E22" s="20">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F22" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2461,7 +2473,7 @@
       </c>
       <c r="D23" s="19">
         <f t="shared" si="3"/>
-        <v>43151.227766599579</v>
+        <v>43154.075653923537</v>
       </c>
       <c r="E23" s="20">
         <f t="shared" si="0"/>
@@ -2489,7 +2501,7 @@
       </c>
       <c r="D24" s="19">
         <f t="shared" si="3"/>
-        <v>43152.396378269601</v>
+        <v>43155.311871227357</v>
       </c>
       <c r="E24" s="20">
         <f t="shared" si="0"/>
@@ -2517,7 +2529,7 @@
       </c>
       <c r="D25" s="19">
         <f t="shared" si="3"/>
-        <v>43153.564989939623</v>
+        <v>43156.548088531177</v>
       </c>
       <c r="E25" s="20">
         <f t="shared" si="0"/>
@@ -2545,7 +2557,7 @@
       </c>
       <c r="D26" s="19">
         <f t="shared" si="3"/>
-        <v>43154.733601609645</v>
+        <v>43157.784305834997</v>
       </c>
       <c r="E26" s="20">
         <f t="shared" si="0"/>
@@ -2573,7 +2585,7 @@
       </c>
       <c r="D27" s="19">
         <f t="shared" si="3"/>
-        <v>43160.576659959748</v>
+        <v>43163.965392354112</v>
       </c>
       <c r="E27" s="20">
         <f t="shared" si="0"/>
@@ -2601,11 +2613,11 @@
       </c>
       <c r="D28" s="19">
         <f t="shared" si="3"/>
-        <v>43163.4981891348</v>
+        <v>43167.055935613673</v>
       </c>
       <c r="E28" s="20">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F28" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2629,7 +2641,7 @@
       </c>
       <c r="D29" s="19">
         <f t="shared" si="3"/>
-        <v>43167.004024144859</v>
+        <v>43170.76458752514</v>
       </c>
       <c r="E29" s="20">
         <f t="shared" si="0"/>
@@ -2645,7 +2657,7 @@
         <v/>
       </c>
       <c r="J29" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K29" s="56"/>
     </row>
@@ -2661,7 +2673,7 @@
       </c>
       <c r="D30" s="19">
         <f t="shared" si="3"/>
-        <v>43167.880482897373</v>
+        <v>43171.691750503007</v>
       </c>
       <c r="E30" s="20">
         <f t="shared" si="0"/>
@@ -2677,7 +2689,7 @@
         <v/>
       </c>
       <c r="J30" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K30" s="56"/>
     </row>
@@ -2693,11 +2705,11 @@
       </c>
       <c r="D31" s="19">
         <f t="shared" si="3"/>
-        <v>43168.464788732381</v>
+        <v>43172.309859154921</v>
       </c>
       <c r="E31" s="20">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F31" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2709,7 +2721,7 @@
         <v/>
       </c>
       <c r="J31" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K31" s="56"/>
     </row>
@@ -2725,11 +2737,11 @@
       </c>
       <c r="D32" s="19">
         <f t="shared" si="3"/>
-        <v>43169.633400402403</v>
+        <v>43173.546076458741</v>
       </c>
       <c r="E32" s="20">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F32" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2741,7 +2753,7 @@
         <v/>
       </c>
       <c r="J32" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K32" s="56"/>
     </row>
@@ -2758,11 +2770,11 @@
       </c>
       <c r="D33" s="19">
         <f t="shared" si="3"/>
-        <v>43169.779476861157</v>
+        <v>43173.700603621721</v>
       </c>
       <c r="E33" s="20">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F33" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2774,7 +2786,7 @@
         <v/>
       </c>
       <c r="J33" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K33" s="56"/>
     </row>
@@ -2790,7 +2802,7 @@
       </c>
       <c r="D34" s="19">
         <f t="shared" si="3"/>
-        <v>43173.285311871216</v>
+        <v>43177.409255533188</v>
       </c>
       <c r="E34" s="20">
         <f t="shared" si="0"/>
@@ -2818,7 +2830,7 @@
       </c>
       <c r="D35" s="19">
         <f t="shared" si="3"/>
-        <v>43179.128370221319</v>
+        <v>43183.590342052303</v>
       </c>
       <c r="E35" s="20">
         <f t="shared" ref="E35:E54" si="4">ROUNDDOWN((D35-$M$1)/7, 0)+1</f>
@@ -2846,7 +2858,7 @@
       </c>
       <c r="D36" s="19">
         <f t="shared" si="3"/>
-        <v>43180.881287726348</v>
+        <v>43185.444668008036</v>
       </c>
       <c r="E36" s="20">
         <f t="shared" si="4"/>
@@ -2862,7 +2874,7 @@
         <v/>
       </c>
       <c r="J36" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K36" s="56"/>
     </row>
@@ -2878,11 +2890,11 @@
       </c>
       <c r="D37" s="19">
         <f t="shared" si="3"/>
-        <v>43182.634205231378</v>
+        <v>43187.29899396377</v>
       </c>
       <c r="E37" s="20">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F37" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2894,7 +2906,7 @@
         <v/>
       </c>
       <c r="J37" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K37" s="56"/>
     </row>
@@ -2910,11 +2922,11 @@
       </c>
       <c r="D38" s="19">
         <f t="shared" si="3"/>
-        <v>43184.387122736407</v>
+        <v>43189.153319919504</v>
       </c>
       <c r="E38" s="20">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F38" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2926,7 +2938,7 @@
         <v/>
       </c>
       <c r="J38" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K38" s="56"/>
     </row>
@@ -2942,7 +2954,7 @@
       </c>
       <c r="D39" s="19">
         <f t="shared" si="3"/>
-        <v>43187.892957746466</v>
+        <v>43192.861971830971</v>
       </c>
       <c r="E39" s="20">
         <f t="shared" si="4"/>
@@ -2958,7 +2970,7 @@
         <v/>
       </c>
       <c r="J39" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K39" s="56"/>
     </row>
@@ -2974,11 +2986,11 @@
       </c>
       <c r="D40" s="19">
         <f t="shared" si="3"/>
-        <v>43189.645875251495</v>
+        <v>43194.716297786705</v>
       </c>
       <c r="E40" s="20">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F40" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2990,7 +3002,7 @@
         <v/>
       </c>
       <c r="J40" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K40" s="56"/>
     </row>
@@ -3006,11 +3018,11 @@
       </c>
       <c r="D41" s="19">
         <f t="shared" si="3"/>
-        <v>43190.814486921518</v>
+        <v>43195.952515090525</v>
       </c>
       <c r="E41" s="20">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F41" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3022,7 +3034,7 @@
         <v/>
       </c>
       <c r="J41" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K41" s="56"/>
     </row>
@@ -3038,11 +3050,11 @@
       </c>
       <c r="D42" s="19">
         <f t="shared" si="3"/>
-        <v>43192.567404426547</v>
+        <v>43197.806841046258</v>
       </c>
       <c r="E42" s="20">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F42" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3054,7 +3066,7 @@
         <v/>
       </c>
       <c r="J42" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K42" s="56"/>
     </row>
@@ -3070,7 +3082,7 @@
       </c>
       <c r="D43" s="19">
         <f t="shared" si="3"/>
-        <v>43194.320321931576</v>
+        <v>43199.661167001992</v>
       </c>
       <c r="E43" s="20">
         <f t="shared" si="4"/>
@@ -3086,7 +3098,7 @@
         <v/>
       </c>
       <c r="J43" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K43" s="56"/>
     </row>
@@ -3102,11 +3114,11 @@
       </c>
       <c r="D44" s="19">
         <f t="shared" si="3"/>
-        <v>43196.073239436606</v>
+        <v>43201.515492957726</v>
       </c>
       <c r="E44" s="20">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F44" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3118,7 +3130,7 @@
         <v/>
       </c>
       <c r="J44" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K44" s="56"/>
     </row>
@@ -3134,11 +3146,11 @@
       </c>
       <c r="D45" s="19">
         <f t="shared" si="3"/>
-        <v>43197.241851106628</v>
+        <v>43202.751710261546</v>
       </c>
       <c r="E45" s="20">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F45" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3150,7 +3162,7 @@
         <v/>
       </c>
       <c r="J45" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K45" s="56"/>
     </row>
@@ -3166,11 +3178,11 @@
       </c>
       <c r="D46" s="19">
         <f t="shared" si="3"/>
-        <v>43198.994768611657</v>
+        <v>43204.606036217279</v>
       </c>
       <c r="E46" s="20">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F46" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3182,7 +3194,7 @@
         <v/>
       </c>
       <c r="J46" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K46" s="56"/>
     </row>
@@ -3198,7 +3210,7 @@
       </c>
       <c r="D47" s="19">
         <f t="shared" si="3"/>
-        <v>43200.747686116687</v>
+        <v>43206.460362173013</v>
       </c>
       <c r="E47" s="20">
         <f t="shared" si="4"/>
@@ -3214,7 +3226,7 @@
         <v/>
       </c>
       <c r="J47" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K47" s="56"/>
     </row>
@@ -3230,11 +3242,11 @@
       </c>
       <c r="D48" s="19">
         <f t="shared" si="3"/>
-        <v>43204.253521126746</v>
+        <v>43210.16901408448</v>
       </c>
       <c r="E48" s="20">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F48" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3246,7 +3258,7 @@
         <v/>
       </c>
       <c r="J48" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K48" s="56"/>
     </row>
@@ -3262,11 +3274,11 @@
       </c>
       <c r="D49" s="19">
         <f t="shared" si="3"/>
-        <v>43205.422132796768</v>
+        <v>43211.4052313883</v>
       </c>
       <c r="E49" s="20">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F49" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3278,7 +3290,7 @@
         <v/>
       </c>
       <c r="J49" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K49" s="56"/>
     </row>
@@ -3295,11 +3307,11 @@
       </c>
       <c r="D50" s="19">
         <f t="shared" si="3"/>
-        <v>43208.927967806827</v>
+        <v>43215.113883299768</v>
       </c>
       <c r="E50" s="20">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F50" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3324,11 +3336,11 @@
       </c>
       <c r="D51" s="19">
         <f t="shared" si="3"/>
-        <v>43212.433802816886</v>
+        <v>43218.822535211235</v>
       </c>
       <c r="E51" s="20">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F51" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3353,11 +3365,11 @@
       </c>
       <c r="D52" s="19">
         <f t="shared" si="3"/>
-        <v>43215.939637826945</v>
+        <v>43222.531187122702</v>
       </c>
       <c r="E52" s="20">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F52" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3382,11 +3394,11 @@
       </c>
       <c r="D53" s="19">
         <f t="shared" si="3"/>
-        <v>43219.445472837004</v>
+        <v>43226.23983903417</v>
       </c>
       <c r="E53" s="20">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F53" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3411,11 +3423,11 @@
       </c>
       <c r="D54" s="19">
         <f t="shared" si="3"/>
-        <v>43222.951307847063</v>
+        <v>43229.948490945637</v>
       </c>
       <c r="E54" s="20">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F54" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3427,6 +3439,7 @@
         <v/>
       </c>
     </row>
+    <row r="55" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="49" t="s">
         <v>110</v>
@@ -3436,82 +3449,109 @@
         <v>207.08333333333331</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="49"/>
-    </row>
+    <row r="57" spans="1:11" ht="10.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="49" t="s">
+      <c r="B58" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="44">
+        <f>C56-C59</f>
+        <v>145.58333333333331</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="52">
+        <f>SUM(C50:C54,C34:C35, C27, C23, C11, C4)</f>
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="49"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="C58" s="50">
-        <f>C56-C59</f>
+      <c r="C61" s="50">
+        <f>C56-C62</f>
         <v>37.333333333333314</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="49" t="s">
+      <c r="D61" s="77">
+        <f>C61/$C$56</f>
+        <v>0.180281690140845</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="C59" s="50">
+      <c r="C62" s="50">
         <f>SUMIF(G2:G54, "", C2:C54)</f>
         <v>169.75</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="54" t="s">
+      <c r="D62" s="77">
+        <f>C62/$C$56</f>
+        <v>0.81971830985915506</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="C65" s="44">
+        <f>C58*0.6</f>
+        <v>87.34999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" s="52">
+        <f>+C59</f>
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="C62" s="52">
-        <f>SUM(C50:C54,C34:C35, C27, C23, C11, C4)</f>
-        <v>61.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="51" t="s">
+      <c r="C68" s="46">
+        <f>+C65+C66</f>
+        <v>148.84999999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="49"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="C63" s="44">
-        <f>C56-C62</f>
-        <v>145.58333333333331</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="C64" s="44">
-        <f>C63*0.6</f>
-        <v>87.34999999999998</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="49" t="s">
+      <c r="C70" s="50">
+        <f>C61</f>
+        <v>37.333333333333314</v>
+      </c>
+      <c r="D70" s="77">
+        <f>C70/$C$68</f>
+        <v>0.25081177919605863</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="C66" s="46">
-        <f>C62+C64</f>
-        <v>148.84999999999997</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="49"/>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="49" t="s">
-        <v>121</v>
-      </c>
-      <c r="C68" s="50">
-        <f>C58</f>
-        <v>37.333333333333314</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="C69" s="50">
-        <f>C66-C68</f>
+      <c r="C71" s="50">
+        <f>C68-C70</f>
         <v>111.51666666666665</v>
+      </c>
+      <c r="D71" s="77">
+        <f>C71/$C$68</f>
+        <v>0.74918822080394143</v>
       </c>
     </row>
   </sheetData>
@@ -3528,10 +3568,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
   <dimension ref="A1:R57"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C56" sqref="C56"/>
       <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
@@ -5119,10 +5163,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
   <dimension ref="O1:P4"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
completed ch 2 of 5 - Manipulating DataFrames with pandas - DataCamp
</commit_message>
<xml_diff>
--- a/Springboard Course Schedule & Study Plan.xlsx
+++ b/Springboard Course Schedule & Study Plan.xlsx
@@ -1838,14 +1838,14 @@
       </c>
       <c r="K4" s="39">
         <f ca="1">K5*7</f>
-        <v>13.979411764705883</v>
+        <v>14.490853658536587</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>121</v>
       </c>
       <c r="M4" s="39">
         <f ca="1">M5*7</f>
-        <v>9.1837254901960765</v>
+        <v>9.5197154471544714</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1882,14 +1882,14 @@
       </c>
       <c r="K5" s="39">
         <f ca="1">C62/(M2-TODAY())</f>
-        <v>1.9970588235294118</v>
+        <v>2.0701219512195124</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>122</v>
       </c>
       <c r="M5" s="39">
         <f ca="1">C71/(M2-TODAY())</f>
-        <v>1.3119607843137253</v>
+        <v>1.3599593495934958</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1956,14 +1956,14 @@
       </c>
       <c r="K7" s="39">
         <f ca="1">+K4*1.5</f>
-        <v>20.969117647058823</v>
+        <v>21.73628048780488</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>128</v>
       </c>
       <c r="M7" s="39">
         <f ca="1">+M4*1.5</f>
-        <v>13.775588235294116</v>
+        <v>14.279573170731707</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2000,14 +2000,14 @@
       </c>
       <c r="K8" s="39">
         <f ca="1">+K5*1.5</f>
-        <v>2.9955882352941177</v>
+        <v>3.1051829268292686</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>129</v>
       </c>
       <c r="M8" s="39">
         <f ca="1">+M5*1.5</f>
-        <v>1.9679411764705881</v>
+        <v>2.039939024390244</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="F18" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SOON</v>
+        <v>DUE</v>
       </c>
       <c r="G18" s="59"/>
       <c r="H18" s="47">
@@ -2369,12 +2369,12 @@
       </c>
       <c r="F19" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>DUE</v>
       </c>
       <c r="G19" s="59"/>
-      <c r="H19" s="47" t="str">
+      <c r="H19" s="47">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2397,12 +2397,12 @@
       </c>
       <c r="F20" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>SOON</v>
       </c>
       <c r="G20" s="59"/>
-      <c r="H20" s="47" t="str">
+      <c r="H20" s="47">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>